<commit_message>
Main struct of Armors selector
</commit_message>
<xml_diff>
--- a/Personnage.xlsx
+++ b/Personnage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -1250,7 +1250,7 @@
     <numFmt numFmtId="172" formatCode="&quot;+ &quot;General"/>
     <numFmt numFmtId="173" formatCode="&quot;/ &quot;General&quot; Kg&quot;"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1996,101 +1996,68 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2107,6 +2074,14 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="171" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2123,79 +2098,104 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -3054,6 +3054,7 @@
       <sheetName val="Races"/>
       <sheetName val="Sous-races"/>
       <sheetName val="Classes"/>
+      <sheetName val="Capacities"/>
       <sheetName val="Historiques"/>
       <sheetName val="Armes"/>
       <sheetName val="Armures"/>
@@ -3064,6 +3065,7 @@
       <sheetName val="Services"/>
       <sheetName val="Babioles"/>
       <sheetName val="Equipements"/>
+      <sheetName val="Feuil1"/>
       <sheetName val="Génasis"/>
       <sheetName val="Moine"/>
     </sheetNames>
@@ -3294,7 +3296,8 @@
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6">
         <row r="2">
           <cell r="A2" t="str">
             <v>Armes courantes de corps à corps</v>
@@ -4053,7 +4056,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
@@ -4063,6 +4065,8 @@
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4392,7 +4396,7 @@
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.5703125" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
@@ -4410,14 +4414,14 @@
     <col min="15" max="15" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="187" t="s">
+      <c r="C1" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="187"/>
+      <c r="D1" s="201"/>
       <c r="E1" s="93" t="s">
         <v>325</v>
       </c>
@@ -4430,22 +4434,22 @@
       <c r="H1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="192" t="s">
+      <c r="I1" s="183" t="s">
         <v>270</v>
       </c>
-      <c r="J1" s="192"/>
+      <c r="J1" s="183"/>
       <c r="K1" s="3"/>
       <c r="L1" s="79"/>
       <c r="M1" s="79"/>
     </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15">
       <c r="B2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="186" t="s">
+      <c r="C2" s="200" t="s">
         <v>301</v>
       </c>
-      <c r="D2" s="186"/>
+      <c r="D2" s="200"/>
       <c r="E2" s="22" t="s">
         <v>324</v>
       </c>
@@ -4459,39 +4463,39 @@
       <c r="H2" s="45">
         <v>0</v>
       </c>
-      <c r="I2" s="193">
+      <c r="I2" s="206">
         <f>VLOOKUP($G$2+1,[1]Niveaux!$A$2:$C$21,2)</f>
         <v>300</v>
       </c>
-      <c r="J2" s="193"/>
-      <c r="K2" s="206"/>
-      <c r="L2" s="206"/>
-      <c r="M2" s="207"/>
-    </row>
-    <row r="3" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="206"/>
+      <c r="K2" s="161"/>
+      <c r="L2" s="161"/>
+      <c r="M2" s="162"/>
+    </row>
+    <row r="3" spans="2:15" ht="11.25" customHeight="1">
       <c r="K3" s="102"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
+    <row r="4" spans="2:15">
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
       <c r="E4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="189" t="s">
+      <c r="H4" s="203" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="189"/>
-      <c r="J4" s="189"/>
+      <c r="I4" s="203"/>
+      <c r="J4" s="203"/>
       <c r="K4" s="145"/>
-      <c r="L4" s="192" t="s">
+      <c r="L4" s="183" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="192"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M4" s="183"/>
+    </row>
+    <row r="5" spans="2:15">
       <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
@@ -4515,7 +4519,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15">
       <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
@@ -4541,7 +4545,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
@@ -4567,7 +4571,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
@@ -4591,7 +4595,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
@@ -4615,11 +4619,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="196" t="s">
+    <row r="10" spans="2:15">
+      <c r="C10" s="188" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="197"/>
+      <c r="D10" s="189"/>
       <c r="E10" s="64">
         <v>14</v>
       </c>
@@ -4639,10 +4643,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="K11" s="102"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
@@ -4661,11 +4665,11 @@
       <c r="K12" s="144"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="196" t="s">
+    <row r="13" spans="2:15">
+      <c r="C13" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="D13" s="197"/>
+      <c r="D13" s="189"/>
       <c r="E13" s="40"/>
       <c r="F13" s="10"/>
       <c r="G13" s="12"/>
@@ -4675,7 +4679,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" ht="15.75" thickBot="1">
       <c r="B14" s="31"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
@@ -4691,7 +4695,7 @@
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="C16" s="15" t="s">
         <v>20</v>
       </c>
@@ -4709,17 +4713,17 @@
         <v>25</v>
       </c>
       <c r="I16" s="14"/>
-      <c r="L16" s="218" t="s">
+      <c r="L16" s="180" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="218"/>
-      <c r="N16" s="218"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C17" s="190">
+      <c r="M16" s="180"/>
+      <c r="N16" s="180"/>
+    </row>
+    <row r="17" spans="3:14">
+      <c r="C17" s="204">
         <v>11</v>
       </c>
-      <c r="D17" s="191"/>
+      <c r="D17" s="205"/>
       <c r="E17" s="109"/>
       <c r="F17" s="110"/>
       <c r="G17" s="110"/>
@@ -4728,12 +4732,12 @@
       <c r="L17" s="38">
         <v>1</v>
       </c>
-      <c r="M17" s="219" t="s">
+      <c r="M17" s="181" t="s">
         <v>55</v>
       </c>
-      <c r="N17" s="168"/>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N17" s="182"/>
+    </row>
+    <row r="18" spans="3:14">
       <c r="C18" s="103" t="s">
         <v>19</v>
       </c>
@@ -4754,16 +4758,16 @@
       <c r="L18" s="39">
         <v>0</v>
       </c>
-      <c r="M18" s="168" t="s">
+      <c r="M18" s="182" t="s">
         <v>56</v>
       </c>
-      <c r="N18" s="168"/>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="194">
+      <c r="N18" s="182"/>
+    </row>
+    <row r="19" spans="3:14">
+      <c r="C19" s="186">
         <v>10</v>
       </c>
-      <c r="D19" s="195"/>
+      <c r="D19" s="187"/>
       <c r="E19" s="106">
         <v>10</v>
       </c>
@@ -4781,41 +4785,41 @@
       <c r="L19" s="39">
         <v>0</v>
       </c>
-      <c r="M19" s="168" t="s">
+      <c r="M19" s="182" t="s">
         <v>57</v>
       </c>
-      <c r="N19" s="168"/>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="182"/>
+    </row>
+    <row r="20" spans="3:14">
       <c r="C20" s="114" t="s">
         <v>327</v>
       </c>
       <c r="D20" s="115"/>
-      <c r="E20" s="203" t="s">
+      <c r="E20" s="197" t="s">
         <v>328</v>
       </c>
-      <c r="F20" s="203"/>
+      <c r="F20" s="197"/>
       <c r="G20" s="141" t="s">
         <v>365</v>
       </c>
       <c r="L20" s="39">
         <v>0</v>
       </c>
-      <c r="M20" s="168" t="s">
+      <c r="M20" s="182" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="168"/>
-    </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="194">
-        <v>0</v>
-      </c>
-      <c r="D21" s="195"/>
-      <c r="E21" s="200" t="str">
+      <c r="N20" s="182"/>
+    </row>
+    <row r="21" spans="3:14">
+      <c r="C21" s="186">
+        <v>0</v>
+      </c>
+      <c r="D21" s="187"/>
+      <c r="E21" s="194" t="str">
         <f>VLOOKUP($G$2,Classe!$A$3:$F$22,4)</f>
         <v>-</v>
       </c>
-      <c r="F21" s="200"/>
+      <c r="F21" s="194"/>
       <c r="G21" s="142" t="str">
         <f>VLOOKUP($G$2,Classe!A3:G22,7)</f>
         <v>-</v>
@@ -4823,244 +4827,244 @@
       <c r="L21" s="40">
         <v>0</v>
       </c>
-      <c r="M21" s="220" t="s">
+      <c r="M21" s="184" t="s">
         <v>59</v>
       </c>
-      <c r="N21" s="221"/>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N21" s="185"/>
+    </row>
+    <row r="22" spans="3:14">
       <c r="C22" s="116"/>
       <c r="D22" s="116"/>
       <c r="E22" s="116"/>
     </row>
-    <row r="24" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:14" ht="15" customHeight="1">
       <c r="C24" s="89" t="s">
         <v>285</v>
       </c>
       <c r="D24" s="89"/>
-      <c r="E24" s="208" t="s">
+      <c r="E24" s="163" t="s">
         <v>261</v>
       </c>
-      <c r="F24" s="208"/>
-      <c r="G24" s="208"/>
+      <c r="F24" s="163"/>
+      <c r="G24" s="163"/>
       <c r="J24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K24" s="209" t="s">
+      <c r="K24" s="164" t="s">
         <v>64</v>
       </c>
-      <c r="L24" s="210"/>
-      <c r="M24" s="210"/>
-      <c r="N24" s="211"/>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L24" s="165"/>
+      <c r="M24" s="165"/>
+      <c r="N24" s="166"/>
+    </row>
+    <row r="25" spans="3:14">
       <c r="C25" s="155" t="s">
         <v>329</v>
       </c>
       <c r="D25" s="156" t="s">
         <v>362</v>
       </c>
-      <c r="E25" s="201"/>
-      <c r="F25" s="201"/>
-      <c r="G25" s="202"/>
+      <c r="E25" s="195"/>
+      <c r="F25" s="195"/>
+      <c r="G25" s="196"/>
       <c r="J25" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="K25" s="181"/>
-      <c r="L25" s="182"/>
-      <c r="M25" s="182"/>
-      <c r="N25" s="183"/>
-    </row>
-    <row r="26" spans="3:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="167"/>
+      <c r="L25" s="168"/>
+      <c r="M25" s="168"/>
+      <c r="N25" s="169"/>
+    </row>
+    <row r="26" spans="3:14" ht="14.25" customHeight="1">
       <c r="C26" s="157" t="s">
         <v>329</v>
       </c>
       <c r="D26" s="158" t="s">
         <v>361</v>
       </c>
-      <c r="E26" s="184" t="str">
+      <c r="E26" s="178" t="str">
         <f>VLOOKUP($G$2,Classe!A3:F22,3,FALSE)</f>
         <v>1d4</v>
       </c>
-      <c r="F26" s="184"/>
-      <c r="G26" s="185"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="179"/>
       <c r="J26" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="K26" s="179" t="str">
+      <c r="K26" s="170" t="str">
         <f>VLOOKUP($K24,[1]Armes!$A$2:$F$42,3)</f>
         <v>1d6 contondant</v>
       </c>
-      <c r="L26" s="180"/>
-      <c r="M26" s="180"/>
+      <c r="L26" s="171"/>
+      <c r="M26" s="171"/>
       <c r="N26" s="120">
         <f>IF(IFERROR(INDEX(Maitrise!$A$2:$B$40,MATCH($K$24,Maitrise!$B$2:$B$40,0),1),0)=1,Maitrise!$P$2,"")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:14" ht="15" customHeight="1">
       <c r="C27" s="157" t="s">
         <v>329</v>
       </c>
       <c r="D27" s="158" t="s">
         <v>281</v>
       </c>
-      <c r="E27" s="184" t="s">
+      <c r="E27" s="178" t="s">
         <v>283</v>
       </c>
-      <c r="F27" s="184"/>
-      <c r="G27" s="185"/>
-      <c r="J27" s="169" t="s">
+      <c r="F27" s="178"/>
+      <c r="G27" s="179"/>
+      <c r="J27" s="207" t="s">
         <v>158</v>
       </c>
-      <c r="K27" s="212" t="str">
+      <c r="K27" s="172" t="str">
         <f>VLOOKUP($K24,[1]Armes!$A$2:$F$42,4,FALSE)&amp;" - "&amp;VLOOKUP($K24,[1]Armes!$A$2:$F$42,6,FALSE)</f>
         <v>2 kg - Polyvalente (1d8)</v>
       </c>
-      <c r="L27" s="213"/>
-      <c r="M27" s="213"/>
-      <c r="N27" s="214"/>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L27" s="173"/>
+      <c r="M27" s="173"/>
+      <c r="N27" s="174"/>
+    </row>
+    <row r="28" spans="3:14">
       <c r="C28" s="159">
         <v>1</v>
       </c>
       <c r="D28" s="158" t="s">
         <v>282</v>
       </c>
-      <c r="E28" s="184" t="s">
+      <c r="E28" s="178" t="s">
         <v>326</v>
       </c>
-      <c r="F28" s="184"/>
-      <c r="G28" s="185"/>
-      <c r="J28" s="170"/>
-      <c r="K28" s="212"/>
-      <c r="L28" s="213"/>
-      <c r="M28" s="213"/>
-      <c r="N28" s="214"/>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F28" s="178"/>
+      <c r="G28" s="179"/>
+      <c r="J28" s="208"/>
+      <c r="K28" s="172"/>
+      <c r="L28" s="173"/>
+      <c r="M28" s="173"/>
+      <c r="N28" s="174"/>
+    </row>
+    <row r="29" spans="3:14">
       <c r="C29" s="39"/>
       <c r="D29" s="85"/>
-      <c r="E29" s="184"/>
-      <c r="F29" s="184"/>
-      <c r="G29" s="185"/>
-      <c r="J29" s="171"/>
-      <c r="K29" s="215"/>
-      <c r="L29" s="216"/>
-      <c r="M29" s="216"/>
-      <c r="N29" s="217"/>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E29" s="178"/>
+      <c r="F29" s="178"/>
+      <c r="G29" s="179"/>
+      <c r="J29" s="209"/>
+      <c r="K29" s="175"/>
+      <c r="L29" s="176"/>
+      <c r="M29" s="176"/>
+      <c r="N29" s="177"/>
+    </row>
+    <row r="30" spans="3:14">
       <c r="C30" s="39"/>
       <c r="D30" s="85"/>
-      <c r="E30" s="184"/>
-      <c r="F30" s="184"/>
-      <c r="G30" s="185"/>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E30" s="178"/>
+      <c r="F30" s="178"/>
+      <c r="G30" s="179"/>
+    </row>
+    <row r="31" spans="3:14">
       <c r="C31" s="39"/>
       <c r="D31" s="85"/>
-      <c r="E31" s="184"/>
-      <c r="F31" s="184"/>
-      <c r="G31" s="185"/>
+      <c r="E31" s="178"/>
+      <c r="F31" s="178"/>
+      <c r="G31" s="179"/>
       <c r="J31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K31" s="209" t="s">
+      <c r="K31" s="164" t="s">
         <v>330</v>
       </c>
-      <c r="L31" s="210"/>
-      <c r="M31" s="210"/>
-      <c r="N31" s="211"/>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L31" s="165"/>
+      <c r="M31" s="165"/>
+      <c r="N31" s="166"/>
+    </row>
+    <row r="32" spans="3:14">
       <c r="C32" s="39"/>
       <c r="D32" s="85"/>
-      <c r="E32" s="184"/>
-      <c r="F32" s="184"/>
-      <c r="G32" s="185"/>
+      <c r="E32" s="178"/>
+      <c r="F32" s="178"/>
+      <c r="G32" s="179"/>
       <c r="J32" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="K32" s="181"/>
-      <c r="L32" s="182"/>
-      <c r="M32" s="182"/>
-      <c r="N32" s="183"/>
-    </row>
-    <row r="33" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="167"/>
+      <c r="L32" s="168"/>
+      <c r="M32" s="168"/>
+      <c r="N32" s="169"/>
+    </row>
+    <row r="33" spans="3:14" ht="15" customHeight="1">
       <c r="C33" s="39"/>
       <c r="D33" s="85"/>
-      <c r="E33" s="184"/>
-      <c r="F33" s="184"/>
-      <c r="G33" s="185"/>
+      <c r="E33" s="178"/>
+      <c r="F33" s="178"/>
+      <c r="G33" s="179"/>
       <c r="J33" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="K33" s="179" t="str">
+      <c r="K33" s="170" t="str">
         <f>VLOOKUP($K31,[1]Armes!$A$2:$F$42,3)</f>
         <v>1d4 tranchant</v>
       </c>
-      <c r="L33" s="180"/>
-      <c r="M33" s="180"/>
+      <c r="L33" s="171"/>
+      <c r="M33" s="171"/>
       <c r="N33" s="120">
         <f>IF(IFERROR(INDEX(Maitrise!$A$2:$B$40,MATCH($K$31,Maitrise!$B$2:$B$40,0),1),0)=1,Maitrise!$P$2,"")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="3:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:14" ht="16.5" customHeight="1">
       <c r="C34" s="39"/>
       <c r="D34" s="85"/>
-      <c r="E34" s="184"/>
-      <c r="F34" s="184"/>
-      <c r="G34" s="185"/>
+      <c r="E34" s="178"/>
+      <c r="F34" s="178"/>
+      <c r="G34" s="179"/>
       <c r="J34" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="K34" s="178">
+      <c r="K34" s="216">
         <v>10</v>
       </c>
-      <c r="L34" s="163"/>
-      <c r="M34" s="163"/>
-      <c r="N34" s="164"/>
-    </row>
-    <row r="35" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L34" s="192"/>
+      <c r="M34" s="192"/>
+      <c r="N34" s="193"/>
+    </row>
+    <row r="35" spans="3:14" ht="15" customHeight="1">
       <c r="C35" s="39"/>
       <c r="D35" s="85"/>
-      <c r="E35" s="184"/>
-      <c r="F35" s="184"/>
-      <c r="G35" s="185"/>
-      <c r="J35" s="169" t="s">
+      <c r="E35" s="178"/>
+      <c r="F35" s="178"/>
+      <c r="G35" s="179"/>
+      <c r="J35" s="207" t="s">
         <v>158</v>
       </c>
-      <c r="K35" s="172" t="str">
+      <c r="K35" s="210" t="str">
         <f>VLOOKUP($K31,[1]Armes!$A$2:$F$42,4,FALSE)&amp;" - "&amp;VLOOKUP($K31,[1]Armes!$A$2:$F$42,6,FALSE)</f>
         <v>0 g - Munitions (portée 9 m/36 m)</v>
       </c>
-      <c r="L35" s="173"/>
-      <c r="M35" s="173"/>
-      <c r="N35" s="174"/>
-    </row>
-    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="L35" s="211"/>
+      <c r="M35" s="211"/>
+      <c r="N35" s="212"/>
+    </row>
+    <row r="36" spans="3:14">
       <c r="C36" s="40"/>
       <c r="D36" s="83"/>
-      <c r="E36" s="204"/>
-      <c r="F36" s="204"/>
-      <c r="G36" s="205"/>
-      <c r="J36" s="170"/>
-      <c r="K36" s="172"/>
-      <c r="L36" s="173"/>
-      <c r="M36" s="173"/>
-      <c r="N36" s="174"/>
-    </row>
-    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="J37" s="171"/>
-      <c r="K37" s="175"/>
-      <c r="L37" s="176"/>
-      <c r="M37" s="176"/>
-      <c r="N37" s="177"/>
-    </row>
-    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E36" s="198"/>
+      <c r="F36" s="198"/>
+      <c r="G36" s="199"/>
+      <c r="J36" s="208"/>
+      <c r="K36" s="210"/>
+      <c r="L36" s="211"/>
+      <c r="M36" s="211"/>
+      <c r="N36" s="212"/>
+    </row>
+    <row r="37" spans="3:14">
+      <c r="J37" s="209"/>
+      <c r="K37" s="213"/>
+      <c r="L37" s="214"/>
+      <c r="M37" s="214"/>
+      <c r="N37" s="215"/>
+    </row>
+    <row r="38" spans="3:14">
       <c r="C38" s="95" t="s">
         <v>160</v>
       </c>
@@ -5072,212 +5076,256 @@
       <c r="G38" s="153"/>
       <c r="M38" s="94"/>
     </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:14">
       <c r="C39" s="98"/>
       <c r="D39" s="96">
         <v>0</v>
       </c>
-      <c r="E39" s="198"/>
-      <c r="F39" s="198"/>
-      <c r="G39" s="199"/>
+      <c r="E39" s="190"/>
+      <c r="F39" s="190"/>
+      <c r="G39" s="191"/>
       <c r="J39" s="154"/>
-      <c r="K39" s="165"/>
-      <c r="L39" s="165"/>
-      <c r="M39" s="165"/>
-      <c r="N39" s="165"/>
-    </row>
-    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="K39" s="219"/>
+      <c r="L39" s="219"/>
+      <c r="M39" s="219"/>
+      <c r="N39" s="219"/>
+    </row>
+    <row r="40" spans="3:14">
       <c r="C40" s="99"/>
       <c r="D40" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="E40" s="163"/>
-      <c r="F40" s="163"/>
-      <c r="G40" s="164"/>
+      <c r="E40" s="192"/>
+      <c r="F40" s="192"/>
+      <c r="G40" s="193"/>
       <c r="J40" s="154"/>
-      <c r="K40" s="167"/>
-      <c r="L40" s="167"/>
-      <c r="M40" s="167"/>
-      <c r="N40" s="167"/>
-    </row>
-    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="K40" s="221"/>
+      <c r="L40" s="221"/>
+      <c r="M40" s="221"/>
+      <c r="N40" s="221"/>
+    </row>
+    <row r="41" spans="3:14">
       <c r="C41" s="99"/>
       <c r="D41" s="97" t="s">
         <v>161</v>
       </c>
-      <c r="E41" s="163"/>
-      <c r="F41" s="163"/>
-      <c r="G41" s="164"/>
+      <c r="E41" s="192"/>
+      <c r="F41" s="192"/>
+      <c r="G41" s="193"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="154"/>
-      <c r="K41" s="166"/>
-      <c r="L41" s="166"/>
-      <c r="M41" s="166"/>
-      <c r="N41" s="166"/>
-    </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="K41" s="220"/>
+      <c r="L41" s="220"/>
+      <c r="M41" s="220"/>
+      <c r="N41" s="220"/>
+    </row>
+    <row r="42" spans="3:14">
       <c r="C42" s="99"/>
       <c r="D42" s="97" t="s">
         <v>166</v>
       </c>
-      <c r="E42" s="163"/>
-      <c r="F42" s="163"/>
-      <c r="G42" s="164"/>
-    </row>
-    <row r="43" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E42" s="192"/>
+      <c r="F42" s="192"/>
+      <c r="G42" s="193"/>
+    </row>
+    <row r="43" spans="3:14">
       <c r="C43" s="99"/>
       <c r="D43" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="E43" s="163"/>
-      <c r="F43" s="163"/>
-      <c r="G43" s="164"/>
-    </row>
-    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E43" s="192"/>
+      <c r="F43" s="192"/>
+      <c r="G43" s="193"/>
+    </row>
+    <row r="44" spans="3:14">
       <c r="C44" s="99"/>
       <c r="D44" s="97" t="s">
         <v>167</v>
       </c>
-      <c r="E44" s="163"/>
-      <c r="F44" s="163"/>
-      <c r="G44" s="164"/>
-    </row>
-    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E44" s="192"/>
+      <c r="F44" s="192"/>
+      <c r="G44" s="193"/>
+    </row>
+    <row r="45" spans="3:14">
       <c r="C45" s="99"/>
       <c r="D45" s="97" t="s">
         <v>164</v>
       </c>
-      <c r="E45" s="163"/>
-      <c r="F45" s="163"/>
-      <c r="G45" s="164"/>
-    </row>
-    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E45" s="192"/>
+      <c r="F45" s="192"/>
+      <c r="G45" s="193"/>
+    </row>
+    <row r="46" spans="3:14">
       <c r="C46" s="100"/>
       <c r="D46" s="97" t="s">
         <v>168</v>
       </c>
-      <c r="E46" s="163"/>
-      <c r="F46" s="163"/>
-      <c r="G46" s="164"/>
-    </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E46" s="192"/>
+      <c r="F46" s="192"/>
+      <c r="G46" s="193"/>
+    </row>
+    <row r="47" spans="3:14">
       <c r="C47" s="99"/>
       <c r="D47" s="97" t="s">
         <v>165</v>
       </c>
-      <c r="E47" s="163"/>
-      <c r="F47" s="163"/>
-      <c r="G47" s="164"/>
-    </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="E47" s="192"/>
+      <c r="F47" s="192"/>
+      <c r="G47" s="193"/>
+    </row>
+    <row r="48" spans="3:14">
       <c r="C48" s="99"/>
       <c r="D48" s="97" t="s">
         <v>169</v>
       </c>
-      <c r="E48" s="163"/>
-      <c r="F48" s="163"/>
-      <c r="G48" s="164"/>
-    </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="E48" s="192"/>
+      <c r="F48" s="192"/>
+      <c r="G48" s="193"/>
+    </row>
+    <row r="49" spans="3:15">
       <c r="C49" s="99"/>
       <c r="D49" s="147"/>
-      <c r="E49" s="163"/>
-      <c r="F49" s="163"/>
-      <c r="G49" s="164"/>
-    </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="E49" s="192"/>
+      <c r="F49" s="192"/>
+      <c r="G49" s="193"/>
+    </row>
+    <row r="50" spans="3:15">
       <c r="C50" s="101"/>
       <c r="D50" s="160"/>
-      <c r="E50" s="161"/>
-      <c r="F50" s="161"/>
-      <c r="G50" s="162"/>
-    </row>
-    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="E50" s="217"/>
+      <c r="F50" s="217"/>
+      <c r="G50" s="218"/>
+    </row>
+    <row r="56" spans="3:15">
       <c r="I56" s="146"/>
       <c r="L56" s="12"/>
       <c r="M56" s="12"/>
       <c r="N56" s="12"/>
       <c r="O56" s="12"/>
     </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:15">
       <c r="I57" s="147"/>
       <c r="L57" s="12"/>
       <c r="M57" s="12"/>
       <c r="N57" s="12"/>
       <c r="O57" s="12"/>
     </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:15">
       <c r="I58" s="148"/>
       <c r="L58" s="12"/>
       <c r="M58" s="12"/>
       <c r="N58" s="12"/>
       <c r="O58" s="12"/>
     </row>
-    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:15">
       <c r="I59" s="149"/>
       <c r="L59" s="151"/>
       <c r="M59" s="152"/>
       <c r="N59" s="12"/>
       <c r="O59" s="12"/>
     </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:15">
       <c r="I60" s="149"/>
       <c r="L60" s="12"/>
       <c r="M60" s="12"/>
       <c r="N60" s="12"/>
       <c r="O60" s="12"/>
     </row>
-    <row r="61" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:15">
       <c r="I61" s="149"/>
       <c r="L61" s="12"/>
       <c r="M61" s="12"/>
       <c r="N61" s="12"/>
       <c r="O61" s="12"/>
     </row>
-    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:15">
       <c r="L62" s="12"/>
       <c r="M62" s="12"/>
       <c r="N62" s="12"/>
       <c r="O62" s="12"/>
     </row>
-    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:15">
       <c r="I63" s="146"/>
       <c r="L63" s="12"/>
       <c r="M63" s="12"/>
       <c r="N63" s="12"/>
       <c r="O63" s="12"/>
     </row>
-    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:15">
       <c r="I64" s="147"/>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:9">
       <c r="I65" s="148"/>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="9:9">
       <c r="I66" s="147"/>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="9:9">
       <c r="I67" s="150"/>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="9:9">
       <c r="I68" s="150"/>
     </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="9:9">
       <c r="I69" s="150"/>
     </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="9:9">
       <c r="I71" s="146"/>
     </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="9:9">
       <c r="I72" s="147"/>
     </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="9:9">
       <c r="I73" s="148"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" scenarios="1"/>
   <mergeCells count="60">
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="K35:N37"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="K24:N24"/>
@@ -5294,50 +5342,6 @@
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:G28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="K35:N37"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="J35:J37"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="K39:N39"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:I10">
     <cfRule type="expression" dxfId="9" priority="27">
@@ -5544,13 +5548,13 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -5558,7 +5562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -5566,7 +5570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -5574,7 +5578,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -5582,7 +5586,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -5590,7 +5594,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -5598,7 +5602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -5606,7 +5610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -5614,7 +5618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
         <v>271</v>
       </c>
@@ -5622,7 +5626,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="4" t="s">
         <v>274</v>
       </c>
@@ -5630,7 +5634,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="4" t="s">
         <v>275</v>
       </c>
@@ -5638,7 +5642,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
         <v>277</v>
       </c>
@@ -5646,7 +5650,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="134.25" customHeight="1">
       <c r="A16" s="87" t="s">
         <v>210</v>
       </c>
@@ -5654,7 +5658,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="222" t="s">
         <v>37</v>
       </c>
@@ -5662,13 +5666,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="222"/>
       <c r="B19" s="48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="222"/>
       <c r="B20" s="52" t="s">
         <v>284</v>
@@ -5691,7 +5695,7 @@
       <selection activeCell="C2" sqref="C2:C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
@@ -5715,7 +5719,7 @@
     <col min="20" max="20" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="81"/>
       <c r="B1" s="82" t="s">
         <v>60</v>
@@ -5745,7 +5749,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -5788,7 +5792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="39">
         <v>1</v>
       </c>
@@ -5827,7 +5831,7 @@
       </c>
       <c r="O3" s="12"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="39">
         <v>1</v>
       </c>
@@ -5866,7 +5870,7 @@
       </c>
       <c r="O4" s="12"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="39">
         <v>1</v>
       </c>
@@ -5899,7 +5903,7 @@
       </c>
       <c r="O5" s="12"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="39">
         <v>1</v>
       </c>
@@ -5930,7 +5934,7 @@
       </c>
       <c r="O6" s="12"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="39">
         <v>1</v>
       </c>
@@ -5961,7 +5965,7 @@
       </c>
       <c r="O7" s="12"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="39">
         <v>1</v>
       </c>
@@ -5992,7 +5996,7 @@
       </c>
       <c r="O8" s="12"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="39">
         <v>1</v>
       </c>
@@ -6023,7 +6027,7 @@
       </c>
       <c r="O9" s="12"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="39">
         <v>1</v>
       </c>
@@ -6054,7 +6058,7 @@
       </c>
       <c r="O10" s="12"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="39">
         <v>1</v>
       </c>
@@ -6083,7 +6087,7 @@
       </c>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="118"/>
       <c r="B12" s="119" t="s">
         <v>62</v>
@@ -6108,7 +6112,7 @@
       </c>
       <c r="O12" s="12"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="38">
         <v>0</v>
       </c>
@@ -6135,7 +6139,7 @@
       </c>
       <c r="O13" s="12"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="39">
         <v>0</v>
       </c>
@@ -6162,7 +6166,7 @@
       </c>
       <c r="O14" s="12"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="39">
         <v>0</v>
       </c>
@@ -6189,7 +6193,7 @@
       </c>
       <c r="O15" s="12"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="39">
         <v>1</v>
       </c>
@@ -6214,7 +6218,7 @@
       </c>
       <c r="O16" s="12"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="39">
         <v>0</v>
       </c>
@@ -6241,7 +6245,7 @@
       </c>
       <c r="O17" s="12"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="39">
         <v>0</v>
       </c>
@@ -6268,7 +6272,7 @@
       </c>
       <c r="O18" s="12"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="39">
         <v>0</v>
       </c>
@@ -6295,7 +6299,7 @@
       </c>
       <c r="O19" s="12"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="39">
         <v>0</v>
       </c>
@@ -6307,7 +6311,7 @@
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="39">
         <v>0</v>
       </c>
@@ -6319,7 +6323,7 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="39">
         <v>0</v>
       </c>
@@ -6331,7 +6335,7 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" s="39">
         <v>0</v>
       </c>
@@ -6343,7 +6347,7 @@
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" s="39">
         <v>0</v>
       </c>
@@ -6355,7 +6359,7 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="39">
         <v>0</v>
       </c>
@@ -6367,7 +6371,7 @@
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="39">
         <v>0</v>
       </c>
@@ -6379,7 +6383,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="39">
         <v>0</v>
       </c>
@@ -6391,7 +6395,7 @@
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="39">
         <v>0</v>
       </c>
@@ -6403,7 +6407,7 @@
       <c r="N28" s="12"/>
       <c r="O28" s="12"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" s="39">
         <v>0</v>
       </c>
@@ -6415,7 +6419,7 @@
       <c r="N29" s="117"/>
       <c r="O29" s="12"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="32"/>
       <c r="B30" s="82" t="s">
         <v>61</v>
@@ -6425,7 +6429,7 @@
       <c r="N30" s="117"/>
       <c r="O30" s="12"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="38">
         <v>1</v>
       </c>
@@ -6437,7 +6441,7 @@
       <c r="N31" s="117"/>
       <c r="O31" s="12"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="39">
         <v>1</v>
       </c>
@@ -6449,7 +6453,7 @@
       <c r="N32" s="117"/>
       <c r="O32" s="12"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="39">
         <v>1</v>
       </c>
@@ -6461,7 +6465,7 @@
       <c r="N33" s="117"/>
       <c r="O33" s="12"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="39">
         <v>1</v>
       </c>
@@ -6473,7 +6477,7 @@
       <c r="N34" s="117"/>
       <c r="O34" s="12"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="32"/>
       <c r="B35" s="82" t="s">
         <v>63</v>
@@ -6483,7 +6487,7 @@
       <c r="N35" s="117"/>
       <c r="O35" s="12"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="38">
         <v>0</v>
       </c>
@@ -6495,7 +6499,7 @@
       <c r="N36" s="117"/>
       <c r="O36" s="12"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="39">
         <v>0</v>
       </c>
@@ -6507,7 +6511,7 @@
       <c r="N37" s="117"/>
       <c r="O37" s="12"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="39">
         <v>0</v>
       </c>
@@ -6519,7 +6523,7 @@
       <c r="N38" s="117"/>
       <c r="O38" s="12"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="39">
         <v>0</v>
       </c>
@@ -6531,7 +6535,7 @@
       <c r="N39" s="117"/>
       <c r="O39" s="12"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" s="40">
         <v>0</v>
       </c>
@@ -6543,19 +6547,19 @@
       <c r="N40" s="117"/>
       <c r="O40" s="12"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="L41" s="117"/>
       <c r="M41" s="12"/>
       <c r="N41" s="117"/>
       <c r="O41" s="12"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="L42" s="117"/>
       <c r="M42" s="12"/>
       <c r="N42" s="117"/>
       <c r="O42" s="12"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="L43" s="117"/>
       <c r="M43" s="12"/>
       <c r="N43" s="117"/>
@@ -6670,28 +6674,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="223" t="s">
         <v>171</v>
       </c>
       <c r="B1" s="224"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -6704,16 +6708,16 @@
       <c r="D2" t="str">
         <f>""""&amp;B2&amp;""": {  ""Caracteristic"": """&amp;LEFT(RIGHT(C2,4),3)&amp;""",
   ""Name"": """&amp;B2&amp;"""
- },"</f>
+ }"</f>
         <v>"Acrobatie": {  "Caracteristic": "DEX",
   "Name": "Acrobatie"
- },</v>
+ }</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="39">
         <v>0</v>
       </c>
@@ -6726,16 +6730,16 @@
       <c r="D3" t="str">
         <f t="shared" ref="D3:D66" si="0">""""&amp;B3&amp;""": {  ""Caracteristic"": """&amp;LEFT(RIGHT(C3,4),3)&amp;""",
   ""Name"": """&amp;B3&amp;"""
- },"</f>
+ }"</f>
         <v>"Ambidextrie": {  "Caracteristic": "DEX",
   "Name": "Ambidextrie"
- },</v>
+ }</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="39">
         <v>0</v>
       </c>
@@ -6749,13 +6753,13 @@
         <f t="shared" si="0"/>
         <v>"Apnée": {  "Caracteristic": "CON",
   "Name": "Apnée"
- },</v>
+ }</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="39">
         <v>0</v>
       </c>
@@ -6769,13 +6773,13 @@
         <f t="shared" si="0"/>
         <v>"Arnaque": {  "Caracteristic": "INT",
   "Name": "Arnaque"
- },</v>
+ }</v>
       </c>
       <c r="I5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="39">
         <v>0</v>
       </c>
@@ -6789,13 +6793,13 @@
         <f t="shared" si="0"/>
         <v>"Arcane": {  "Caracteristic": "INT",
   "Name": "Arcane"
- },</v>
+ }</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="39">
         <v>0</v>
       </c>
@@ -6809,13 +6813,13 @@
         <f t="shared" si="0"/>
         <v>"Assasinat": {  "Caracteristic": "DEX",
   "Name": "Assasinat"
- },</v>
+ }</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="39">
         <v>0</v>
       </c>
@@ -6829,13 +6833,13 @@
         <f t="shared" si="0"/>
         <v>"Athlétisme": {  "Caracteristic": "FOR",
   "Name": "Athlétisme"
- },</v>
+ }</v>
       </c>
       <c r="I8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="39">
         <v>0</v>
       </c>
@@ -6849,13 +6853,13 @@
         <f t="shared" si="0"/>
         <v>"Audition": {  "Caracteristic": "SAG",
   "Name": "Audition"
- },</v>
+ }</v>
       </c>
       <c r="I9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="39">
         <v>0</v>
       </c>
@@ -6869,13 +6873,13 @@
         <f t="shared" si="0"/>
         <v>"Bagarre": {  "Caracteristic": "FOR",
   "Name": "Bagarre"
- },</v>
+ }</v>
       </c>
       <c r="I10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="39">
         <v>0</v>
       </c>
@@ -6889,13 +6893,13 @@
         <f t="shared" si="0"/>
         <v>"Baratineur": {  "Caracteristic": "CHA",
   "Name": "Baratineur"
- },</v>
+ }</v>
       </c>
       <c r="I11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="39">
         <v>0</v>
       </c>
@@ -6909,13 +6913,13 @@
         <f t="shared" si="0"/>
         <v>"Bravoure": {  "Caracteristic": "CHA",
   "Name": "Bravoure"
- },</v>
+ }</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="39">
         <v>0</v>
       </c>
@@ -6929,13 +6933,13 @@
         <f t="shared" si="0"/>
         <v>"Bricolage": {  "Caracteristic": "INT",
   "Name": "Bricolage"
- },</v>
+ }</v>
       </c>
       <c r="I13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="39">
         <v>0</v>
       </c>
@@ -6949,13 +6953,13 @@
         <f t="shared" si="0"/>
         <v>"Brise liens": {  "Caracteristic": "CON",
   "Name": "Brise liens"
- },</v>
+ }</v>
       </c>
       <c r="I14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="39">
         <v>0</v>
       </c>
@@ -6969,13 +6973,13 @@
         <f t="shared" si="0"/>
         <v>"Chance": {  "Caracteristic": "SAG",
   "Name": "Chance"
- },</v>
+ }</v>
       </c>
       <c r="I15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="39">
         <v>0</v>
       </c>
@@ -6989,13 +6993,13 @@
         <f t="shared" si="0"/>
         <v>"Chasse": {  "Caracteristic": "SAG",
   "Name": "Chasse"
- },</v>
+ }</v>
       </c>
       <c r="I16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="39">
         <v>0</v>
       </c>
@@ -7009,13 +7013,13 @@
         <f t="shared" si="0"/>
         <v>"Matrise des nœuds": {  "Caracteristic": "INT",
   "Name": "Matrise des nœuds"
- },</v>
+ }</v>
       </c>
       <c r="I17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="39">
         <v>0</v>
       </c>
@@ -7029,13 +7033,13 @@
         <f t="shared" si="0"/>
         <v>"Corruption": {  "Caracteristic": "INT",
   "Name": "Corruption"
- },</v>
+ }</v>
       </c>
       <c r="I18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="39">
         <v>0</v>
       </c>
@@ -7049,13 +7053,13 @@
         <f t="shared" si="0"/>
         <v>"Crochetage": {  "Caracteristic": "DEX",
   "Name": "Crochetage"
- },</v>
+ }</v>
       </c>
       <c r="I19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="39">
         <v>0</v>
       </c>
@@ -7069,13 +7073,13 @@
         <f t="shared" si="0"/>
         <v>"(Dé)cryptage": {  "Caracteristic": "INT",
   "Name": "(Dé)cryptage"
- },</v>
+ }</v>
       </c>
       <c r="I20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="39">
         <v>0</v>
       </c>
@@ -7089,13 +7093,13 @@
         <f t="shared" si="0"/>
         <v>"Cuisine": {  "Caracteristic": "INT",
   "Name": "Cuisine"
- },</v>
+ }</v>
       </c>
       <c r="I21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="39">
         <v>0</v>
       </c>
@@ -7109,13 +7113,13 @@
         <f t="shared" si="0"/>
         <v>"Déguisement": {  "Caracteristic": "CHA",
   "Name": "Déguisement"
- },</v>
+ }</v>
       </c>
       <c r="I22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="39">
         <v>0</v>
       </c>
@@ -7129,13 +7133,13 @@
         <f t="shared" si="0"/>
         <v>"Désamorçage": {  "Caracteristic": "SAG",
   "Name": "Désamorçage"
- },</v>
+ }</v>
       </c>
       <c r="I23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="39">
         <v>0</v>
       </c>
@@ -7149,13 +7153,13 @@
         <f t="shared" si="0"/>
         <v>"Détection d'émotions": {  "Caracteristic": "SAG",
   "Name": "Détection d'émotions"
- },</v>
+ }</v>
       </c>
       <c r="I24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="39">
         <v>0</v>
       </c>
@@ -7169,13 +7173,13 @@
         <f t="shared" si="0"/>
         <v>"Diplomatie": {  "Caracteristic": "CHA",
   "Name": "Diplomatie"
- },</v>
+ }</v>
       </c>
       <c r="I25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="39">
         <v>1</v>
       </c>
@@ -7189,13 +7193,13 @@
         <f t="shared" si="0"/>
         <v>"Discrétion": {  "Caracteristic": "DEX",
   "Name": "Discrétion"
- },</v>
+ }</v>
       </c>
       <c r="I26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="39">
         <v>0</v>
       </c>
@@ -7209,13 +7213,13 @@
         <f t="shared" si="0"/>
         <v>"Dissimulation": {  "Caracteristic": "DEX",
   "Name": "Dissimulation"
- },</v>
+ }</v>
       </c>
       <c r="I27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="39">
         <v>0</v>
       </c>
@@ -7229,13 +7233,13 @@
         <f t="shared" si="0"/>
         <v>"Donjonnerie": {  "Caracteristic": "INT",
   "Name": "Donjonnerie"
- },</v>
+ }</v>
       </c>
       <c r="I28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="39">
         <v>0</v>
       </c>
@@ -7249,13 +7253,13 @@
         <f t="shared" si="0"/>
         <v>"Dressage": {  "Caracteristic": "SAG",
   "Name": "Dressage"
- },</v>
+ }</v>
       </c>
       <c r="I29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="39">
         <v>0</v>
       </c>
@@ -7269,13 +7273,13 @@
         <f t="shared" si="0"/>
         <v>"Eloquence": {  "Caracteristic": "CHA",
   "Name": "Eloquence"
- },</v>
+ }</v>
       </c>
       <c r="I30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="39">
         <v>0</v>
       </c>
@@ -7289,13 +7293,13 @@
         <f t="shared" si="0"/>
         <v>"Equilibre": {  "Caracteristic": "DEX",
   "Name": "Equilibre"
- },</v>
+ }</v>
       </c>
       <c r="I31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="39">
         <v>0</v>
       </c>
@@ -7309,13 +7313,13 @@
         <f t="shared" si="0"/>
         <v>"Escalade": {  "Caracteristic": "CON",
   "Name": "Escalade"
- },</v>
+ }</v>
       </c>
       <c r="I32">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="39">
         <v>0</v>
       </c>
@@ -7329,13 +7333,13 @@
         <f t="shared" si="0"/>
         <v>"Escamotage": {  "Caracteristic": "DEX",
   "Name": "Escamotage"
- },</v>
+ }</v>
       </c>
       <c r="I33">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="39">
         <v>0</v>
       </c>
@@ -7349,13 +7353,13 @@
         <f t="shared" si="0"/>
         <v>"Espionnage": {  "Caracteristic": "SAG",
   "Name": "Espionnage"
- },</v>
+ }</v>
       </c>
       <c r="I34">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="39">
         <v>0</v>
       </c>
@@ -7369,13 +7373,13 @@
         <f t="shared" si="0"/>
         <v>"Estimation": {  "Caracteristic": "INT",
   "Name": "Estimation"
- },</v>
+ }</v>
       </c>
       <c r="I35">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="39">
         <v>0</v>
       </c>
@@ -7389,13 +7393,13 @@
         <f t="shared" si="0"/>
         <v>"Etiquette": {  "Caracteristic": "CON",
   "Name": "Etiquette"
- },</v>
+ }</v>
       </c>
       <c r="I36">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="39">
         <v>0</v>
       </c>
@@ -7409,13 +7413,13 @@
         <f t="shared" si="0"/>
         <v>"Exploration": {  "Caracteristic": "SAG",
   "Name": "Exploration"
- },</v>
+ }</v>
       </c>
       <c r="I37">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="39">
         <v>0</v>
       </c>
@@ -7429,13 +7433,13 @@
         <f t="shared" si="0"/>
         <v>"Fouille": {  "Caracteristic": "SAG",
   "Name": "Fouille"
- },</v>
+ }</v>
       </c>
       <c r="I38">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="39">
         <v>0</v>
       </c>
@@ -7449,13 +7453,13 @@
         <f t="shared" si="0"/>
         <v>"Fuite": {  "Caracteristic": "CON",
   "Name": "Fuite"
- },</v>
+ }</v>
       </c>
       <c r="I39">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="39">
         <v>0</v>
       </c>
@@ -7469,13 +7473,13 @@
         <f t="shared" si="0"/>
         <v>"Géographie": {  "Caracteristic": "INT",
   "Name": "Géographie"
- },</v>
+ }</v>
       </c>
       <c r="I40">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="39">
         <v>0</v>
       </c>
@@ -7489,13 +7493,13 @@
         <f t="shared" si="0"/>
         <v>"Herboristerie": {  "Caracteristic": "SAG",
   "Name": "Herboristerie"
- },</v>
+ }</v>
       </c>
       <c r="I41">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="39">
         <v>0</v>
       </c>
@@ -7509,13 +7513,13 @@
         <f t="shared" si="0"/>
         <v>"Histoire": {  "Caracteristic": "INT",
   "Name": "Histoire"
- },</v>
+ }</v>
       </c>
       <c r="I42">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="39">
         <v>0</v>
       </c>
@@ -7529,13 +7533,13 @@
         <f t="shared" si="0"/>
         <v>"Identification": {  "Caracteristic": "INT",
   "Name": "Identification"
- },</v>
+ }</v>
       </c>
       <c r="I43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="39">
         <v>0</v>
       </c>
@@ -7549,13 +7553,13 @@
         <f t="shared" si="0"/>
         <v>"Imitation": {  "Caracteristic": "INT",
   "Name": "Imitation"
- },</v>
+ }</v>
       </c>
       <c r="I44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="39">
         <v>0</v>
       </c>
@@ -7569,13 +7573,13 @@
         <f t="shared" si="0"/>
         <v>"Intimidation": {  "Caracteristic": "CHA",
   "Name": "Intimidation"
- },</v>
+ }</v>
       </c>
       <c r="I45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="39">
         <v>0</v>
       </c>
@@ -7589,13 +7593,13 @@
         <f t="shared" si="0"/>
         <v>"Intuition": {  "Caracteristic": "SAG",
   "Name": "Intuition"
- },</v>
+ }</v>
       </c>
       <c r="I46">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="39">
         <v>0</v>
       </c>
@@ -7609,13 +7613,13 @@
         <f t="shared" si="0"/>
         <v>"Investigation": {  "Caracteristic": "INT",
   "Name": "Investigation"
- },</v>
+ }</v>
       </c>
       <c r="I47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" s="39">
         <v>0</v>
       </c>
@@ -7629,13 +7633,13 @@
         <f t="shared" si="0"/>
         <v>"Jeu": {  "Caracteristic": "INT",
   "Name": "Jeu"
- },</v>
+ }</v>
       </c>
       <c r="I48">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="39">
         <v>0</v>
       </c>
@@ -7649,13 +7653,13 @@
         <f t="shared" si="0"/>
         <v>"Langue": {  "Caracteristic": "INT",
   "Name": "Langue"
- },</v>
+ }</v>
       </c>
       <c r="I49">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="39">
         <v>0</v>
       </c>
@@ -7669,13 +7673,13 @@
         <f t="shared" si="0"/>
         <v>"Lecture labiale": {  "Caracteristic": "SAG",
   "Name": "Lecture labiale"
- },</v>
+ }</v>
       </c>
       <c r="I50">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="39">
         <v>0</v>
       </c>
@@ -7689,13 +7693,13 @@
         <f t="shared" si="0"/>
         <v>"Loi": {  "Caracteristic": "INT",
   "Name": "Loi"
- },</v>
+ }</v>
       </c>
       <c r="I51">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="39">
         <v>1</v>
       </c>
@@ -7709,13 +7713,13 @@
         <f t="shared" si="0"/>
         <v>"Médecine": {  "Caracteristic": "INT",
   "Name": "Médecine"
- },</v>
+ }</v>
       </c>
       <c r="I52">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="39">
         <v>0</v>
       </c>
@@ -7729,13 +7733,13 @@
         <f t="shared" si="0"/>
         <v>"Méfiance": {  "Caracteristic": "SAG",
   "Name": "Méfiance"
- },</v>
+ }</v>
       </c>
       <c r="I53">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="39">
         <v>0</v>
       </c>
@@ -7749,13 +7753,13 @@
         <f t="shared" si="0"/>
         <v>"Mémorisation": {  "Caracteristic": "INT",
   "Name": "Mémorisation"
- },</v>
+ }</v>
       </c>
       <c r="I54">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="39">
         <v>0</v>
       </c>
@@ -7769,13 +7773,13 @@
         <f t="shared" si="0"/>
         <v>"Narcotique": {  "Caracteristic": "INT",
   "Name": "Narcotique"
- },</v>
+ }</v>
       </c>
       <c r="I55">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" s="39">
         <v>0</v>
       </c>
@@ -7789,13 +7793,13 @@
         <f t="shared" si="0"/>
         <v>"Natation": {  "Caracteristic": "FOR",
   "Name": "Natation"
- },</v>
+ }</v>
       </c>
       <c r="I56">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="39">
         <v>0</v>
       </c>
@@ -7809,13 +7813,13 @@
         <f t="shared" si="0"/>
         <v>"Nature": {  "Caracteristic": "INT",
   "Name": "Nature"
- },</v>
+ }</v>
       </c>
       <c r="I57">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="39">
         <v>0</v>
       </c>
@@ -7829,13 +7833,13 @@
         <f t="shared" si="0"/>
         <v>"Navigation": {  "Caracteristic": "INT",
   "Name": "Navigation"
- },</v>
+ }</v>
       </c>
       <c r="I58">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="39">
         <v>0</v>
       </c>
@@ -7849,13 +7853,13 @@
         <f t="shared" si="0"/>
         <v>"Négociation": {  "Caracteristic": "CHA",
   "Name": "Négociation"
- },</v>
+ }</v>
       </c>
       <c r="I59">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" s="39">
         <v>0</v>
       </c>
@@ -7869,13 +7873,13 @@
         <f t="shared" si="0"/>
         <v>"Noblesse": {  "Caracteristic": "INT",
   "Name": "Noblesse"
- },</v>
+ }</v>
       </c>
       <c r="I60">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="39">
         <v>0</v>
       </c>
@@ -7889,13 +7893,13 @@
         <f t="shared" si="0"/>
         <v>"Noyade": {  "Caracteristic": "CON",
   "Name": "Noyade"
- },</v>
+ }</v>
       </c>
       <c r="I61">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" s="39">
         <v>0</v>
       </c>
@@ -7909,13 +7913,13 @@
         <f t="shared" si="0"/>
         <v>"Observation": {  "Caracteristic": "SAG",
   "Name": "Observation"
- },</v>
+ }</v>
       </c>
       <c r="I62">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63" s="39">
         <v>0</v>
       </c>
@@ -7929,13 +7933,13 @@
         <f t="shared" si="0"/>
         <v>"Odorat": {  "Caracteristic": "SAG",
   "Name": "Odorat"
- },</v>
+ }</v>
       </c>
       <c r="I63">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" s="39">
         <v>0</v>
       </c>
@@ -7949,13 +7953,13 @@
         <f t="shared" si="0"/>
         <v>"Orientation": {  "Caracteristic": "SAG",
   "Name": "Orientation"
- },</v>
+ }</v>
       </c>
       <c r="I64">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9">
       <c r="A65" s="39">
         <v>0</v>
       </c>
@@ -7969,13 +7973,13 @@
         <f t="shared" si="0"/>
         <v>"Pêche": {  "Caracteristic": "SAG",
   "Name": "Pêche"
- },</v>
+ }</v>
       </c>
       <c r="I65">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9">
       <c r="A66" s="39">
         <v>0</v>
       </c>
@@ -7989,13 +7993,13 @@
         <f t="shared" si="0"/>
         <v>"Perspicacité": {  "Caracteristic": "SAG",
   "Name": "Perspicacité"
- },</v>
+ }</v>
       </c>
       <c r="I66">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9">
       <c r="A67" s="39">
         <v>0</v>
       </c>
@@ -8006,18 +8010,18 @@
         <v>252</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D80" si="1">""""&amp;B67&amp;""": {  ""Caracteristic"": """&amp;LEFT(RIGHT(C67,4),3)&amp;""",
+        <f t="shared" ref="D67:D81" si="1">""""&amp;B67&amp;""": {  ""Caracteristic"": """&amp;LEFT(RIGHT(C67,4),3)&amp;""",
   ""Name"": """&amp;B67&amp;"""
- },"</f>
+ }"</f>
         <v>"Persuasion": {  "Caracteristic": "CHA",
   "Name": "Persuasion"
- },</v>
+ }</v>
       </c>
       <c r="I67">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9">
       <c r="A68" s="39">
         <v>0</v>
       </c>
@@ -8031,13 +8035,13 @@
         <f t="shared" si="1"/>
         <v>"Pistage": {  "Caracteristic": "SAG",
   "Name": "Pistage"
- },</v>
+ }</v>
       </c>
       <c r="I68">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9">
       <c r="A69" s="39">
         <v>0</v>
       </c>
@@ -8051,13 +8055,13 @@
         <f t="shared" si="1"/>
         <v>"Poison": {  "Caracteristic": "INT",
   "Name": "Poison"
- },</v>
+ }</v>
       </c>
       <c r="I69">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9">
       <c r="A70" s="39">
         <v>0</v>
       </c>
@@ -8071,13 +8075,13 @@
         <f t="shared" si="1"/>
         <v>"Premiers secours": {  "Caracteristic": "INT",
   "Name": "Premiers secours"
- },</v>
+ }</v>
       </c>
       <c r="I70">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9">
       <c r="A71" s="39">
         <v>0</v>
       </c>
@@ -8091,13 +8095,13 @@
         <f t="shared" si="1"/>
         <v>"Réflexe": {  "Caracteristic": "DEX",
   "Name": "Réflexe"
- },</v>
+ }</v>
       </c>
       <c r="I71">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9">
       <c r="A72" s="39">
         <v>1</v>
       </c>
@@ -8111,13 +8115,13 @@
         <f t="shared" si="1"/>
         <v>"Religion": {  "Caracteristic": "INT",
   "Name": "Religion"
- },</v>
+ }</v>
       </c>
       <c r="I72">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9">
       <c r="A73" s="39">
         <v>0</v>
       </c>
@@ -8131,13 +8135,13 @@
         <f t="shared" si="1"/>
         <v>"Représentation": {  "Caracteristic": "CHA",
   "Name": "Représentation"
- },</v>
+ }</v>
       </c>
       <c r="I73">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9">
       <c r="A74" s="39">
         <v>0</v>
       </c>
@@ -8151,13 +8155,13 @@
         <f t="shared" si="1"/>
         <v>"Sabotage": {  "Caracteristic": "SAG",
   "Name": "Sabotage"
- },</v>
+ }</v>
       </c>
       <c r="I74">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9">
       <c r="A75" s="39">
         <v>0</v>
       </c>
@@ -8171,13 +8175,13 @@
         <f t="shared" si="1"/>
         <v>"Saut": {  "Caracteristic": "FOR",
   "Name": "Saut"
- },</v>
+ }</v>
       </c>
       <c r="I75">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9">
       <c r="A76" s="39">
         <v>0</v>
       </c>
@@ -8191,13 +8195,13 @@
         <f t="shared" si="1"/>
         <v>"Soin animaux": {  "Caracteristic": "SAG",
   "Name": "Soin animaux"
- },</v>
+ }</v>
       </c>
       <c r="I76">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9">
       <c r="A77" s="39">
         <v>0</v>
       </c>
@@ -8211,13 +8215,13 @@
         <f t="shared" si="1"/>
         <v>"Suffocation": {  "Caracteristic": "CON",
   "Name": "Suffocation"
- },</v>
+ }</v>
       </c>
       <c r="I77">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9">
       <c r="A78" s="39">
         <v>0</v>
       </c>
@@ -8231,13 +8235,13 @@
         <f t="shared" si="1"/>
         <v>"Torture": {  "Caracteristic": "CON",
   "Name": "Torture"
- },</v>
+ }</v>
       </c>
       <c r="I78">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9">
       <c r="A79" s="39">
         <v>0</v>
       </c>
@@ -8251,13 +8255,13 @@
         <f t="shared" si="1"/>
         <v>"Tromperie": {  "Caracteristic": "CHA",
   "Name": "Tromperie"
- },</v>
+ }</v>
       </c>
       <c r="I79">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9">
       <c r="A80" s="39">
         <v>0</v>
       </c>
@@ -8271,13 +8275,13 @@
         <f t="shared" si="1"/>
         <v>"Utilisation d'objets magiques": {  "Caracteristic": "INT",
   "Name": "Utilisation d'objets magiques"
- },</v>
+ }</v>
       </c>
       <c r="I80">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9">
       <c r="A81" s="40">
         <v>0</v>
       </c>
@@ -8288,15 +8292,337 @@
         <v>251</v>
       </c>
       <c r="D81" t="str">
-        <f>""""&amp;B81&amp;""": {  ""Caracteristic"": """&amp;LEFT(RIGHT(C81,4),3)&amp;""",
-  ""Name"": """&amp;B81&amp;"""
- },"</f>
+        <f t="shared" si="1"/>
         <v>"Vigilance": {  "Caracteristic": "SAG",
   "Name": "Vigilance"
- },</v>
+ }</v>
       </c>
       <c r="I81">
         <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="D83" t="str">
+        <f>CONCATENATE(D2,",
+",D3,",
+",D4,",
+",D5,",
+",D6,",
+",D7,",
+",D8,",
+",D9,",
+",D10,",
+",D11,",
+",D12,",
+",D13,",
+",D14,",
+",D15,",
+",D16,",
+",D17,",
+",D18,",
+",D19,",
+",D20,",
+",D21,",
+",D22,",
+",D23,",
+",D24,",
+",D25,",
+",D26,",
+",D27,",
+",D28,",
+",D29,",
+",D30,",
+",D31,",
+",D32,",
+",D33,",
+",D34,",
+",D35,",
+",D36,",
+",D37,",
+",D38,",
+",D39,",
+",D40,",
+",D41,",
+",D42,",
+",D43,",
+",D44,",
+",D45,",
+",D46,",
+",D47,",
+",D48,",
+",D49,",
+",D50,",
+",D51,",
+",D52,",
+",D53,",
+",D54,",
+",D55,",
+",D56,",
+",D57,",
+",D58,",
+",D59,",
+",D60,",
+",D61,",
+",D62,",
+",D63,",
+",D64,",
+",D65,",
+",D66,",
+",D67,",
+",D68,",
+",D69,",
+",D70,",
+",D71,",
+",D72,",
+",D73,",
+",D74,",
+",D75,",
+",D76,",
+",D77,",
+",D78,",
+",D79,",
+",D80,",
+",D81)</f>
+        <v>"Acrobatie": {  "Caracteristic": "DEX",
+  "Name": "Acrobatie"
+ },
+"Ambidextrie": {  "Caracteristic": "DEX",
+  "Name": "Ambidextrie"
+ },
+"Apnée": {  "Caracteristic": "CON",
+  "Name": "Apnée"
+ },
+"Arnaque": {  "Caracteristic": "INT",
+  "Name": "Arnaque"
+ },
+"Arcane": {  "Caracteristic": "INT",
+  "Name": "Arcane"
+ },
+"Assasinat": {  "Caracteristic": "DEX",
+  "Name": "Assasinat"
+ },
+"Athlétisme": {  "Caracteristic": "FOR",
+  "Name": "Athlétisme"
+ },
+"Audition": {  "Caracteristic": "SAG",
+  "Name": "Audition"
+ },
+"Bagarre": {  "Caracteristic": "FOR",
+  "Name": "Bagarre"
+ },
+"Baratineur": {  "Caracteristic": "CHA",
+  "Name": "Baratineur"
+ },
+"Bravoure": {  "Caracteristic": "CHA",
+  "Name": "Bravoure"
+ },
+"Bricolage": {  "Caracteristic": "INT",
+  "Name": "Bricolage"
+ },
+"Brise liens": {  "Caracteristic": "CON",
+  "Name": "Brise liens"
+ },
+"Chance": {  "Caracteristic": "SAG",
+  "Name": "Chance"
+ },
+"Chasse": {  "Caracteristic": "SAG",
+  "Name": "Chasse"
+ },
+"Matrise des nœuds": {  "Caracteristic": "INT",
+  "Name": "Matrise des nœuds"
+ },
+"Corruption": {  "Caracteristic": "INT",
+  "Name": "Corruption"
+ },
+"Crochetage": {  "Caracteristic": "DEX",
+  "Name": "Crochetage"
+ },
+"(Dé)cryptage": {  "Caracteristic": "INT",
+  "Name": "(Dé)cryptage"
+ },
+"Cuisine": {  "Caracteristic": "INT",
+  "Name": "Cuisine"
+ },
+"Déguisement": {  "Caracteristic": "CHA",
+  "Name": "Déguisement"
+ },
+"Désamorçage": {  "Caracteristic": "SAG",
+  "Name": "Désamorçage"
+ },
+"Détection d'émotions": {  "Caracteristic": "SAG",
+  "Name": "Détection d'émotions"
+ },
+"Diplomatie": {  "Caracteristic": "CHA",
+  "Name": "Diplomatie"
+ },
+"Discrétion": {  "Caracteristic": "DEX",
+  "Name": "Discrétion"
+ },
+"Dissimulation": {  "Caracteristic": "DEX",
+  "Name": "Dissimulation"
+ },
+"Donjonnerie": {  "Caracteristic": "INT",
+  "Name": "Donjonnerie"
+ },
+"Dressage": {  "Caracteristic": "SAG",
+  "Name": "Dressage"
+ },
+"Eloquence": {  "Caracteristic": "CHA",
+  "Name": "Eloquence"
+ },
+"Equilibre": {  "Caracteristic": "DEX",
+  "Name": "Equilibre"
+ },
+"Escalade": {  "Caracteristic": "CON",
+  "Name": "Escalade"
+ },
+"Escamotage": {  "Caracteristic": "DEX",
+  "Name": "Escamotage"
+ },
+"Espionnage": {  "Caracteristic": "SAG",
+  "Name": "Espionnage"
+ },
+"Estimation": {  "Caracteristic": "INT",
+  "Name": "Estimation"
+ },
+"Etiquette": {  "Caracteristic": "CON",
+  "Name": "Etiquette"
+ },
+"Exploration": {  "Caracteristic": "SAG",
+  "Name": "Exploration"
+ },
+"Fouille": {  "Caracteristic": "SAG",
+  "Name": "Fouille"
+ },
+"Fuite": {  "Caracteristic": "CON",
+  "Name": "Fuite"
+ },
+"Géographie": {  "Caracteristic": "INT",
+  "Name": "Géographie"
+ },
+"Herboristerie": {  "Caracteristic": "SAG",
+  "Name": "Herboristerie"
+ },
+"Histoire": {  "Caracteristic": "INT",
+  "Name": "Histoire"
+ },
+"Identification": {  "Caracteristic": "INT",
+  "Name": "Identification"
+ },
+"Imitation": {  "Caracteristic": "INT",
+  "Name": "Imitation"
+ },
+"Intimidation": {  "Caracteristic": "CHA",
+  "Name": "Intimidation"
+ },
+"Intuition": {  "Caracteristic": "SAG",
+  "Name": "Intuition"
+ },
+"Investigation": {  "Caracteristic": "INT",
+  "Name": "Investigation"
+ },
+"Jeu": {  "Caracteristic": "INT",
+  "Name": "Jeu"
+ },
+"Langue": {  "Caracteristic": "INT",
+  "Name": "Langue"
+ },
+"Lecture labiale": {  "Caracteristic": "SAG",
+  "Name": "Lecture labiale"
+ },
+"Loi": {  "Caracteristic": "INT",
+  "Name": "Loi"
+ },
+"Médecine": {  "Caracteristic": "INT",
+  "Name": "Médecine"
+ },
+"Méfiance": {  "Caracteristic": "SAG",
+  "Name": "Méfiance"
+ },
+"Mémorisation": {  "Caracteristic": "INT",
+  "Name": "Mémorisation"
+ },
+"Narcotique": {  "Caracteristic": "INT",
+  "Name": "Narcotique"
+ },
+"Natation": {  "Caracteristic": "FOR",
+  "Name": "Natation"
+ },
+"Nature": {  "Caracteristic": "INT",
+  "Name": "Nature"
+ },
+"Navigation": {  "Caracteristic": "INT",
+  "Name": "Navigation"
+ },
+"Négociation": {  "Caracteristic": "CHA",
+  "Name": "Négociation"
+ },
+"Noblesse": {  "Caracteristic": "INT",
+  "Name": "Noblesse"
+ },
+"Noyade": {  "Caracteristic": "CON",
+  "Name": "Noyade"
+ },
+"Observation": {  "Caracteristic": "SAG",
+  "Name": "Observation"
+ },
+"Odorat": {  "Caracteristic": "SAG",
+  "Name": "Odorat"
+ },
+"Orientation": {  "Caracteristic": "SAG",
+  "Name": "Orientation"
+ },
+"Pêche": {  "Caracteristic": "SAG",
+  "Name": "Pêche"
+ },
+"Perspicacité": {  "Caracteristic": "SAG",
+  "Name": "Perspicacité"
+ },
+"Persuasion": {  "Caracteristic": "CHA",
+  "Name": "Persuasion"
+ },
+"Pistage": {  "Caracteristic": "SAG",
+  "Name": "Pistage"
+ },
+"Poison": {  "Caracteristic": "INT",
+  "Name": "Poison"
+ },
+"Premiers secours": {  "Caracteristic": "INT",
+  "Name": "Premiers secours"
+ },
+"Réflexe": {  "Caracteristic": "DEX",
+  "Name": "Réflexe"
+ },
+"Religion": {  "Caracteristic": "INT",
+  "Name": "Religion"
+ },
+"Représentation": {  "Caracteristic": "CHA",
+  "Name": "Représentation"
+ },
+"Sabotage": {  "Caracteristic": "SAG",
+  "Name": "Sabotage"
+ },
+"Saut": {  "Caracteristic": "FOR",
+  "Name": "Saut"
+ },
+"Soin animaux": {  "Caracteristic": "SAG",
+  "Name": "Soin animaux"
+ },
+"Suffocation": {  "Caracteristic": "CON",
+  "Name": "Suffocation"
+ },
+"Torture": {  "Caracteristic": "CON",
+  "Name": "Torture"
+ },
+"Tromperie": {  "Caracteristic": "CHA",
+  "Name": "Tromperie"
+ },
+"Utilisation d'objets magiques": {  "Caracteristic": "INT",
+  "Name": "Utilisation d'objets magiques"
+ },
+"Vigilance": {  "Caracteristic": "SAG",
+  "Name": "Vigilance"
+ }</v>
       </c>
     </row>
   </sheetData>
@@ -8348,7 +8674,7 @@
       <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
@@ -8361,7 +8687,7 @@
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="69" t="s">
         <v>257</v>
       </c>
@@ -8393,7 +8719,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="16"/>
       <c r="B2" s="67">
         <v>0</v>
@@ -8410,10 +8736,10 @@
       <c r="F2" s="43">
         <v>0</v>
       </c>
-      <c r="H2" s="233"/>
-      <c r="I2" s="234"/>
-      <c r="J2" s="234"/>
-      <c r="K2" s="235"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="229"/>
+      <c r="J2" s="229"/>
+      <c r="K2" s="230"/>
       <c r="L2" s="67">
         <v>0</v>
       </c>
@@ -8421,249 +8747,279 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="230" t="s">
+      <c r="B3" s="233" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="230"/>
-      <c r="D3" s="230"/>
-      <c r="E3" s="230"/>
-      <c r="F3" s="231"/>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="234"/>
       <c r="H3" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="I3" s="232" t="s">
+      <c r="I3" s="235" t="s">
         <v>261</v>
       </c>
-      <c r="J3" s="232"/>
+      <c r="J3" s="235"/>
       <c r="K3" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="230" t="s">
+      <c r="L3" s="233" t="s">
         <v>261</v>
       </c>
-      <c r="M3" s="231"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" s="234"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="39"/>
-      <c r="B4" s="226"/>
-      <c r="C4" s="226"/>
-      <c r="D4" s="226"/>
-      <c r="E4" s="226"/>
-      <c r="F4" s="227"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="231"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="232"/>
       <c r="H4" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="I4" s="226"/>
-      <c r="J4" s="227"/>
+      <c r="I4" s="231"/>
+      <c r="J4" s="232"/>
       <c r="K4" s="39"/>
-      <c r="L4" s="226"/>
-      <c r="M4" s="227"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L4" s="231"/>
+      <c r="M4" s="232"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="39"/>
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="227"/>
+      <c r="B5" s="231"/>
+      <c r="C5" s="231"/>
+      <c r="D5" s="231"/>
+      <c r="E5" s="231"/>
+      <c r="F5" s="232"/>
       <c r="H5" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="I5" s="226"/>
-      <c r="J5" s="227"/>
+      <c r="I5" s="231"/>
+      <c r="J5" s="232"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="226"/>
-      <c r="M5" s="227"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" s="231"/>
+      <c r="M5" s="232"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="39"/>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="227"/>
+      <c r="B6" s="231"/>
+      <c r="C6" s="231"/>
+      <c r="D6" s="231"/>
+      <c r="E6" s="231"/>
+      <c r="F6" s="232"/>
       <c r="H6" s="39"/>
-      <c r="I6" s="226"/>
-      <c r="J6" s="227"/>
+      <c r="I6" s="231"/>
+      <c r="J6" s="232"/>
       <c r="K6" s="39"/>
-      <c r="L6" s="226"/>
-      <c r="M6" s="227"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" s="231"/>
+      <c r="M6" s="232"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="39"/>
-      <c r="B7" s="226"/>
-      <c r="C7" s="226"/>
-      <c r="D7" s="226"/>
-      <c r="E7" s="226"/>
-      <c r="F7" s="227"/>
+      <c r="B7" s="231"/>
+      <c r="C7" s="231"/>
+      <c r="D7" s="231"/>
+      <c r="E7" s="231"/>
+      <c r="F7" s="232"/>
       <c r="H7" s="39"/>
-      <c r="I7" s="226"/>
-      <c r="J7" s="227"/>
+      <c r="I7" s="231"/>
+      <c r="J7" s="232"/>
       <c r="K7" s="39"/>
-      <c r="L7" s="226"/>
-      <c r="M7" s="227"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L7" s="231"/>
+      <c r="M7" s="232"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="39"/>
-      <c r="B8" s="226"/>
-      <c r="C8" s="226"/>
-      <c r="D8" s="226"/>
-      <c r="E8" s="226"/>
-      <c r="F8" s="227"/>
+      <c r="B8" s="231"/>
+      <c r="C8" s="231"/>
+      <c r="D8" s="231"/>
+      <c r="E8" s="231"/>
+      <c r="F8" s="232"/>
       <c r="H8" s="39"/>
-      <c r="I8" s="226"/>
-      <c r="J8" s="227"/>
+      <c r="I8" s="231"/>
+      <c r="J8" s="232"/>
       <c r="K8" s="75" t="s">
         <v>267</v>
       </c>
-      <c r="L8" s="230" t="s">
+      <c r="L8" s="233" t="s">
         <v>261</v>
       </c>
-      <c r="M8" s="231"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="234"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="39"/>
-      <c r="B9" s="226"/>
-      <c r="C9" s="226"/>
-      <c r="D9" s="226"/>
-      <c r="E9" s="226"/>
-      <c r="F9" s="227"/>
+      <c r="B9" s="231"/>
+      <c r="C9" s="231"/>
+      <c r="D9" s="231"/>
+      <c r="E9" s="231"/>
+      <c r="F9" s="232"/>
       <c r="H9" s="39"/>
-      <c r="I9" s="226"/>
-      <c r="J9" s="227"/>
+      <c r="I9" s="231"/>
+      <c r="J9" s="232"/>
       <c r="K9" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="L9" s="226"/>
-      <c r="M9" s="227"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L9" s="231"/>
+      <c r="M9" s="232"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="39"/>
-      <c r="B10" s="226"/>
-      <c r="C10" s="226"/>
-      <c r="D10" s="226"/>
-      <c r="E10" s="226"/>
-      <c r="F10" s="227"/>
+      <c r="B10" s="231"/>
+      <c r="C10" s="231"/>
+      <c r="D10" s="231"/>
+      <c r="E10" s="231"/>
+      <c r="F10" s="232"/>
       <c r="H10" s="39"/>
-      <c r="I10" s="226"/>
-      <c r="J10" s="227"/>
+      <c r="I10" s="231"/>
+      <c r="J10" s="232"/>
       <c r="K10" s="39"/>
-      <c r="L10" s="226"/>
-      <c r="M10" s="227"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L10" s="231"/>
+      <c r="M10" s="232"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="39"/>
-      <c r="B11" s="226"/>
-      <c r="C11" s="226"/>
-      <c r="D11" s="226"/>
-      <c r="E11" s="226"/>
-      <c r="F11" s="227"/>
+      <c r="B11" s="231"/>
+      <c r="C11" s="231"/>
+      <c r="D11" s="231"/>
+      <c r="E11" s="231"/>
+      <c r="F11" s="232"/>
       <c r="H11" s="39"/>
-      <c r="I11" s="226"/>
-      <c r="J11" s="227"/>
+      <c r="I11" s="231"/>
+      <c r="J11" s="232"/>
       <c r="K11" s="39"/>
-      <c r="L11" s="226"/>
-      <c r="M11" s="227"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L11" s="231"/>
+      <c r="M11" s="232"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="39"/>
-      <c r="B12" s="226"/>
-      <c r="C12" s="226"/>
-      <c r="D12" s="226"/>
-      <c r="E12" s="226"/>
-      <c r="F12" s="227"/>
+      <c r="B12" s="231"/>
+      <c r="C12" s="231"/>
+      <c r="D12" s="231"/>
+      <c r="E12" s="231"/>
+      <c r="F12" s="232"/>
       <c r="H12" s="39"/>
-      <c r="I12" s="226"/>
-      <c r="J12" s="227"/>
+      <c r="I12" s="231"/>
+      <c r="J12" s="232"/>
       <c r="K12" s="39"/>
-      <c r="L12" s="226"/>
-      <c r="M12" s="227"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L12" s="231"/>
+      <c r="M12" s="232"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="39"/>
-      <c r="B13" s="226"/>
-      <c r="C13" s="226"/>
-      <c r="D13" s="226"/>
-      <c r="E13" s="226"/>
-      <c r="F13" s="227"/>
+      <c r="B13" s="231"/>
+      <c r="C13" s="231"/>
+      <c r="D13" s="231"/>
+      <c r="E13" s="231"/>
+      <c r="F13" s="232"/>
       <c r="H13" s="39"/>
-      <c r="I13" s="226"/>
-      <c r="J13" s="227"/>
+      <c r="I13" s="231"/>
+      <c r="J13" s="232"/>
       <c r="K13" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="L13" s="230" t="s">
+      <c r="L13" s="233" t="s">
         <v>261</v>
       </c>
-      <c r="M13" s="231"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="234"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="39"/>
-      <c r="B14" s="226"/>
-      <c r="C14" s="226"/>
-      <c r="D14" s="226"/>
-      <c r="E14" s="226"/>
-      <c r="F14" s="227"/>
+      <c r="B14" s="231"/>
+      <c r="C14" s="231"/>
+      <c r="D14" s="231"/>
+      <c r="E14" s="231"/>
+      <c r="F14" s="232"/>
       <c r="H14" s="39"/>
-      <c r="I14" s="226"/>
-      <c r="J14" s="227"/>
+      <c r="I14" s="231"/>
+      <c r="J14" s="232"/>
       <c r="K14" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="L14" s="226"/>
-      <c r="M14" s="227"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L14" s="231"/>
+      <c r="M14" s="232"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="39"/>
-      <c r="B15" s="226"/>
-      <c r="C15" s="226"/>
-      <c r="D15" s="226"/>
-      <c r="E15" s="226"/>
-      <c r="F15" s="227"/>
+      <c r="B15" s="231"/>
+      <c r="C15" s="231"/>
+      <c r="D15" s="231"/>
+      <c r="E15" s="231"/>
+      <c r="F15" s="232"/>
       <c r="H15" s="39"/>
-      <c r="I15" s="226"/>
-      <c r="J15" s="227"/>
+      <c r="I15" s="231"/>
+      <c r="J15" s="232"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="226"/>
-      <c r="M15" s="227"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L15" s="231"/>
+      <c r="M15" s="232"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="39"/>
-      <c r="B16" s="226"/>
-      <c r="C16" s="226"/>
-      <c r="D16" s="226"/>
-      <c r="E16" s="226"/>
-      <c r="F16" s="227"/>
+      <c r="B16" s="231"/>
+      <c r="C16" s="231"/>
+      <c r="D16" s="231"/>
+      <c r="E16" s="231"/>
+      <c r="F16" s="232"/>
       <c r="H16" s="39"/>
-      <c r="I16" s="226"/>
-      <c r="J16" s="227"/>
+      <c r="I16" s="231"/>
+      <c r="J16" s="232"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="226"/>
-      <c r="M16" s="227"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L16" s="231"/>
+      <c r="M16" s="232"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="40"/>
-      <c r="B17" s="228"/>
-      <c r="C17" s="228"/>
-      <c r="D17" s="228"/>
-      <c r="E17" s="228"/>
-      <c r="F17" s="229"/>
+      <c r="B17" s="226"/>
+      <c r="C17" s="226"/>
+      <c r="D17" s="226"/>
+      <c r="E17" s="226"/>
+      <c r="F17" s="227"/>
       <c r="H17" s="40" t="s">
         <v>265</v>
       </c>
-      <c r="I17" s="228"/>
-      <c r="J17" s="229"/>
+      <c r="I17" s="226"/>
+      <c r="J17" s="227"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="228"/>
-      <c r="M17" s="229"/>
+      <c r="L17" s="226"/>
+      <c r="M17" s="227"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="46">
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="L11:M11"/>
@@ -8680,36 +9036,6 @@
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B16:F16"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
@@ -8738,7 +9064,7 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
@@ -8750,7 +9076,7 @@
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="143" t="s">
         <v>363</v>
       </c>
@@ -8764,7 +9090,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="128" t="s">
         <v>16</v>
       </c>
@@ -8790,7 +9116,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="122">
         <v>1</v>
       </c>
@@ -8816,7 +9142,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="124">
         <v>2</v>
       </c>
@@ -8842,7 +9168,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="122">
         <v>3</v>
       </c>
@@ -8868,7 +9194,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="124">
         <v>4</v>
       </c>
@@ -8894,7 +9220,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="122">
         <v>5</v>
       </c>
@@ -8920,7 +9246,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="124">
         <v>6</v>
       </c>
@@ -8946,7 +9272,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="122">
         <v>7</v>
       </c>
@@ -8972,7 +9298,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="124">
         <v>8</v>
       </c>
@@ -8998,7 +9324,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="122">
         <v>9</v>
       </c>
@@ -9024,7 +9350,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="124">
         <v>10</v>
       </c>
@@ -9050,7 +9376,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="122">
         <v>11</v>
       </c>
@@ -9076,7 +9402,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="124">
         <v>12</v>
       </c>
@@ -9099,7 +9425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="122">
         <v>13</v>
       </c>
@@ -9122,7 +9448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="124">
         <v>14</v>
       </c>
@@ -9145,7 +9471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" s="122">
         <v>15</v>
       </c>
@@ -9168,7 +9494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1">
       <c r="A18" s="124">
         <v>16</v>
       </c>
@@ -9191,7 +9517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1">
       <c r="A19" s="122">
         <v>17</v>
       </c>
@@ -9214,7 +9540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" customHeight="1">
       <c r="A20" s="124">
         <v>18</v>
       </c>
@@ -9237,7 +9563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" customHeight="1">
       <c r="A21" s="122">
         <v>19</v>
       </c>
@@ -9260,7 +9586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" customHeight="1">
       <c r="A22" s="126">
         <v>20</v>
       </c>
@@ -9298,18 +9624,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showRowColHeaders="0" workbookViewId="0">
       <selection activeCell="D1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>297</v>
       </c>
@@ -9317,7 +9643,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>311</v>
       </c>
@@ -9325,7 +9651,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>310</v>
       </c>
@@ -9333,7 +9659,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>309</v>
       </c>
@@ -9341,7 +9667,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>308</v>
       </c>
@@ -9349,7 +9675,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>307</v>
       </c>
@@ -9357,7 +9683,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>306</v>
       </c>
@@ -9365,7 +9691,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>305</v>
       </c>
@@ -9373,7 +9699,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>304</v>
       </c>
@@ -9381,7 +9707,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>299</v>
       </c>
@@ -9389,7 +9715,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>300</v>
       </c>
@@ -9397,23 +9723,23 @@
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="15" customHeight="1"/>
+    <row r="37" ht="15" customHeight="1"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Global Layout + Referential datas (languages, alterations, alignments)
</commit_message>
<xml_diff>
--- a/Personnage.xlsx
+++ b/Personnage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="391">
   <si>
     <t>Nom du personnage</t>
   </si>
@@ -1232,6 +1232,78 @@
   </si>
   <si>
     <t>Force, dextérité</t>
+  </si>
+  <si>
+    <t>Altérations</t>
+  </si>
+  <si>
+    <t>Poisonned</t>
+  </si>
+  <si>
+    <t>Alcoholic</t>
+  </si>
+  <si>
+    <t>Bewitched</t>
+  </si>
+  <si>
+    <t>Scared</t>
+  </si>
+  <si>
+    <t>Provocated</t>
+  </si>
+  <si>
+    <t>Seduced</t>
+  </si>
+  <si>
+    <t>Stressed</t>
+  </si>
+  <si>
+    <t>Acidified</t>
+  </si>
+  <si>
+    <t>Burned</t>
+  </si>
+  <si>
+    <t>Electrified</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>Drug</t>
+  </si>
+  <si>
+    <t>Alcoolisé</t>
+  </si>
+  <si>
+    <t>Envouté</t>
+  </si>
+  <si>
+    <t>Effrayé</t>
+  </si>
+  <si>
+    <t>Provoqué</t>
+  </si>
+  <si>
+    <t>Séduit</t>
+  </si>
+  <si>
+    <t>Stressé</t>
+  </si>
+  <si>
+    <t>Brûlé</t>
+  </si>
+  <si>
+    <t>Foudroyé</t>
+  </si>
+  <si>
+    <t>Drogué</t>
+  </si>
+  <si>
+    <t>Empoisonné</t>
+  </si>
+  <si>
+    <t>Acidifié</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1322,7 @@
     <numFmt numFmtId="172" formatCode="&quot;+ &quot;General"/>
     <numFmt numFmtId="173" formatCode="&quot;/ &quot;General&quot; Kg&quot;"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1383,8 +1455,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1418,6 +1497,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1622,7 +1707,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1996,101 +2081,68 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2107,6 +2159,14 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="171" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2123,85 +2183,169 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2259,64 +2403,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor auto="1"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3065,6 +3151,7 @@
       <sheetName val="Services"/>
       <sheetName val="Babioles"/>
       <sheetName val="Equipements"/>
+      <sheetName val="Sorts"/>
       <sheetName val="Export global"/>
       <sheetName val="Génasis"/>
       <sheetName val="Moine"/>
@@ -3314,13 +3401,13 @@
             <v>1d6 contondant</v>
           </cell>
           <cell r="D3" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>Contondant</v>
+          </cell>
+          <cell r="F3" t="str">
             <v>2 kg</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v>2 pa</v>
-          </cell>
-          <cell r="F3" t="str">
-            <v>Polyvalente (1d8)</v>
           </cell>
         </row>
         <row r="4">
@@ -3334,13 +3421,13 @@
             <v>1d4 perforant</v>
           </cell>
           <cell r="D4" t="str">
+            <v xml:space="preserve">1d4 </v>
+          </cell>
+          <cell r="E4" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F4" t="str">
             <v>500 g</v>
-          </cell>
-          <cell r="E4" t="str">
-            <v>2 po</v>
-          </cell>
-          <cell r="F4" t="str">
-            <v>Finesse, légère, lancer (portée 6 m/18 m)</v>
           </cell>
         </row>
         <row r="5">
@@ -3354,13 +3441,13 @@
             <v>1d4 contondant</v>
           </cell>
           <cell r="D5" t="str">
+            <v xml:space="preserve">1d4 </v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>Contondant</v>
+          </cell>
+          <cell r="F5" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>1 pa</v>
-          </cell>
-          <cell r="F5" t="str">
-            <v>Légère</v>
           </cell>
         </row>
         <row r="6">
@@ -3374,13 +3461,13 @@
             <v>1d6 tranchant</v>
           </cell>
           <cell r="D6" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E6" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F6" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E6" t="str">
-            <v>5 po</v>
-          </cell>
-          <cell r="F6" t="str">
-            <v>Légère, lancer (portée 6 m/18 m)</v>
           </cell>
         </row>
         <row r="7">
@@ -3394,13 +3481,13 @@
             <v>1d6 perforant</v>
           </cell>
           <cell r="D7" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E7" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F7" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E7" t="str">
-            <v>5 pa</v>
-          </cell>
-          <cell r="F7" t="str">
-            <v>Lancer (portée 9 m/36 m)</v>
           </cell>
         </row>
         <row r="8">
@@ -3414,13 +3501,13 @@
             <v>1d6 perforant</v>
           </cell>
           <cell r="D8" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E8" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F8" t="str">
             <v>1,5 kg</v>
-          </cell>
-          <cell r="E8" t="str">
-            <v>1 po</v>
-          </cell>
-          <cell r="F8" t="str">
-            <v>Lancer (portée 6 m/18 m), polyvalente (1d8)</v>
           </cell>
         </row>
         <row r="9">
@@ -3434,13 +3521,13 @@
             <v>1d4 contondant</v>
           </cell>
           <cell r="D9" t="str">
+            <v xml:space="preserve">1d4 </v>
+          </cell>
+          <cell r="E9" t="str">
+            <v>Contondant</v>
+          </cell>
+          <cell r="F9" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E9" t="str">
-            <v>2 po</v>
-          </cell>
-          <cell r="F9" t="str">
-            <v>Légère, lancer (portée 6 m/18 m)</v>
           </cell>
         </row>
         <row r="10">
@@ -3454,13 +3541,13 @@
             <v>1d6 contondant</v>
           </cell>
           <cell r="D10" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E10" t="str">
+            <v>Contondant</v>
+          </cell>
+          <cell r="F10" t="str">
             <v>2 kg</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v>5 po</v>
-          </cell>
-          <cell r="F10" t="str">
-            <v>-</v>
           </cell>
         </row>
         <row r="11">
@@ -3474,13 +3561,13 @@
             <v>1d8 contondant</v>
           </cell>
           <cell r="D11" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E11" t="str">
+            <v>Contondant</v>
+          </cell>
+          <cell r="F11" t="str">
             <v>5 kg</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>2 pa</v>
-          </cell>
-          <cell r="F11" t="str">
-            <v>À deux mains</v>
           </cell>
         </row>
         <row r="12">
@@ -3494,13 +3581,13 @@
             <v>1d4 tranchant</v>
           </cell>
           <cell r="D12" t="str">
+            <v xml:space="preserve">1d4 </v>
+          </cell>
+          <cell r="E12" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F12" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E12" t="str">
-            <v>1 po</v>
-          </cell>
-          <cell r="F12" t="str">
-            <v>Légère</v>
           </cell>
         </row>
         <row r="13">
@@ -3519,13 +3606,13 @@
             <v>1d8 perforant</v>
           </cell>
           <cell r="D14" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E14" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F14" t="str">
             <v>2,5 kg</v>
-          </cell>
-          <cell r="E14" t="str">
-            <v>25 po</v>
-          </cell>
-          <cell r="F14" t="str">
-            <v>Munitions (portée 24 m/96 m), chargement, à deux mains</v>
           </cell>
         </row>
         <row r="15">
@@ -3539,13 +3626,13 @@
             <v>1d6 perforant</v>
           </cell>
           <cell r="D15" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E15" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F15" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E15" t="str">
-            <v>25 po</v>
-          </cell>
-          <cell r="F15" t="str">
-            <v>Munitions (portée 24 m/96 m), à deux mains</v>
           </cell>
         </row>
         <row r="16">
@@ -3559,13 +3646,13 @@
             <v>1d4 perforant</v>
           </cell>
           <cell r="D16" t="str">
+            <v xml:space="preserve">1d4 </v>
+          </cell>
+          <cell r="E16" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F16" t="str">
             <v>100 g</v>
-          </cell>
-          <cell r="E16" t="str">
-            <v>5 pc</v>
-          </cell>
-          <cell r="F16" t="str">
-            <v>Finesse, lancer (portée 6 m/18 m)</v>
           </cell>
         </row>
         <row r="17">
@@ -3579,13 +3666,13 @@
             <v>1d4 contondant</v>
           </cell>
           <cell r="D17" t="str">
+            <v xml:space="preserve">1d4 </v>
+          </cell>
+          <cell r="E17" t="str">
+            <v>Contondant</v>
+          </cell>
+          <cell r="F17" t="str">
             <v>0 g</v>
-          </cell>
-          <cell r="E17" t="str">
-            <v>1 pa</v>
-          </cell>
-          <cell r="F17" t="str">
-            <v>Munitions (portée 9 m/36 m)</v>
           </cell>
         </row>
         <row r="18">
@@ -3604,13 +3691,13 @@
             <v>1d6 tranchant</v>
           </cell>
           <cell r="D19" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E19" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F19" t="str">
             <v>1,5 kg</v>
-          </cell>
-          <cell r="E19" t="str">
-            <v>25 po</v>
-          </cell>
-          <cell r="F19" t="str">
-            <v>Finesse, légère</v>
           </cell>
         </row>
         <row r="20">
@@ -3624,13 +3711,13 @@
             <v>1d10 tranchant</v>
           </cell>
           <cell r="D20" t="str">
+            <v xml:space="preserve">1d10 </v>
+          </cell>
+          <cell r="E20" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F20" t="str">
             <v>3 kg</v>
-          </cell>
-          <cell r="E20" t="str">
-            <v>20 po</v>
-          </cell>
-          <cell r="F20" t="str">
-            <v>Lourde, allonge, à deux mains</v>
           </cell>
         </row>
         <row r="21">
@@ -3644,13 +3731,13 @@
             <v>2d6 tranchant</v>
           </cell>
           <cell r="D21" t="str">
+            <v xml:space="preserve">2d6 </v>
+          </cell>
+          <cell r="E21" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F21" t="str">
             <v>3 kg</v>
-          </cell>
-          <cell r="E21" t="str">
-            <v>50 po</v>
-          </cell>
-          <cell r="F21" t="str">
-            <v>Lourde, à deux mains</v>
           </cell>
         </row>
         <row r="22">
@@ -3664,13 +3751,13 @@
             <v>1d6 perforant</v>
           </cell>
           <cell r="D22" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E22" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F22" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E22" t="str">
-            <v>10 po</v>
-          </cell>
-          <cell r="F22" t="str">
-            <v>Finesse, légère</v>
           </cell>
         </row>
         <row r="23">
@@ -3684,13 +3771,13 @@
             <v>1d8 tranchant</v>
           </cell>
           <cell r="D23" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E23" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F23" t="str">
             <v>1,5 kg</v>
-          </cell>
-          <cell r="E23" t="str">
-            <v>15 po</v>
-          </cell>
-          <cell r="F23" t="str">
-            <v>Polyvalente (1d10)</v>
           </cell>
         </row>
         <row r="24">
@@ -3704,13 +3791,13 @@
             <v>1d8 contondant</v>
           </cell>
           <cell r="D24" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E24" t="str">
+            <v>Contondant</v>
+          </cell>
+          <cell r="F24" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E24" t="str">
-            <v>10 po</v>
-          </cell>
-          <cell r="F24" t="str">
-            <v>-</v>
           </cell>
         </row>
         <row r="25">
@@ -3724,13 +3811,13 @@
             <v>1d4 tranchant</v>
           </cell>
           <cell r="D25" t="str">
+            <v xml:space="preserve">1d4 </v>
+          </cell>
+          <cell r="E25" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F25" t="str">
             <v>1,5 kg</v>
-          </cell>
-          <cell r="E25" t="str">
-            <v>2 po</v>
-          </cell>
-          <cell r="F25" t="str">
-            <v>Finesse, allonge</v>
           </cell>
         </row>
         <row r="26">
@@ -3744,13 +3831,13 @@
             <v>1d12 tranchant</v>
           </cell>
           <cell r="D26" t="str">
+            <v xml:space="preserve">1d12 </v>
+          </cell>
+          <cell r="E26" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F26" t="str">
             <v>3,5 kg</v>
-          </cell>
-          <cell r="E26" t="str">
-            <v>30 po</v>
-          </cell>
-          <cell r="F26" t="str">
-            <v>Lourde, à deux mains</v>
           </cell>
         </row>
         <row r="27">
@@ -3764,13 +3851,13 @@
             <v>1d8 tranchant</v>
           </cell>
           <cell r="D27" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E27" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F27" t="str">
             <v>2 kg</v>
-          </cell>
-          <cell r="E27" t="str">
-            <v>10 po</v>
-          </cell>
-          <cell r="F27" t="str">
-            <v>Polyvalente (1d10)</v>
           </cell>
         </row>
         <row r="28">
@@ -3784,13 +3871,13 @@
             <v>1d10 tranchant</v>
           </cell>
           <cell r="D28" t="str">
+            <v xml:space="preserve">1d10 </v>
+          </cell>
+          <cell r="E28" t="str">
+            <v>Tranchant</v>
+          </cell>
+          <cell r="F28" t="str">
             <v>3 kg</v>
-          </cell>
-          <cell r="E28" t="str">
-            <v>20 po</v>
-          </cell>
-          <cell r="F28" t="str">
-            <v>Lourde, allonge, à deux mains</v>
           </cell>
         </row>
         <row r="29">
@@ -3804,13 +3891,13 @@
             <v>1d12 perforant</v>
           </cell>
           <cell r="D29" t="str">
+            <v xml:space="preserve">1d12 </v>
+          </cell>
+          <cell r="E29" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F29" t="str">
             <v>3 kg</v>
-          </cell>
-          <cell r="E29" t="str">
-            <v>10 po</v>
-          </cell>
-          <cell r="F29" t="str">
-            <v>Allonge, spécial</v>
           </cell>
         </row>
         <row r="30">
@@ -3824,13 +3911,13 @@
             <v>2d6 contondant</v>
           </cell>
           <cell r="D30" t="str">
+            <v xml:space="preserve">2d6 </v>
+          </cell>
+          <cell r="E30" t="str">
+            <v>Contondant</v>
+          </cell>
+          <cell r="F30" t="str">
             <v>5 kg</v>
-          </cell>
-          <cell r="E30" t="str">
-            <v>10 po</v>
-          </cell>
-          <cell r="F30" t="str">
-            <v>Lourde, à deux mains</v>
           </cell>
         </row>
         <row r="31">
@@ -3844,13 +3931,13 @@
             <v>1d8 contondant</v>
           </cell>
           <cell r="D31" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E31" t="str">
+            <v>Contondant</v>
+          </cell>
+          <cell r="F31" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E31" t="str">
-            <v>15 po</v>
-          </cell>
-          <cell r="F31" t="str">
-            <v>Polyvalente (1d10)</v>
           </cell>
         </row>
         <row r="32">
@@ -3864,13 +3951,13 @@
             <v>1d8 perforant</v>
           </cell>
           <cell r="D32" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E32" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F32" t="str">
             <v>2 kg</v>
-          </cell>
-          <cell r="E32" t="str">
-            <v>15 po</v>
-          </cell>
-          <cell r="F32" t="str">
-            <v>-</v>
           </cell>
         </row>
         <row r="33">
@@ -3884,13 +3971,13 @@
             <v>1d8 perforant</v>
           </cell>
           <cell r="D33" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E33" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F33" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E33" t="str">
-            <v>5 po</v>
-          </cell>
-          <cell r="F33" t="str">
-            <v>-</v>
           </cell>
         </row>
         <row r="34">
@@ -3904,13 +3991,13 @@
             <v>1d10 perforant</v>
           </cell>
           <cell r="D34" t="str">
+            <v xml:space="preserve">1d10 </v>
+          </cell>
+          <cell r="E34" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F34" t="str">
             <v>9 kg</v>
-          </cell>
-          <cell r="E34" t="str">
-            <v>5 po</v>
-          </cell>
-          <cell r="F34" t="str">
-            <v>Lourde, allonge, à deux mains</v>
           </cell>
         </row>
         <row r="35">
@@ -3924,13 +4011,13 @@
             <v>1d8 perforant</v>
           </cell>
           <cell r="D35" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E35" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F35" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E35" t="str">
-            <v>25 po</v>
-          </cell>
-          <cell r="F35" t="str">
-            <v>Finesse</v>
           </cell>
         </row>
         <row r="36">
@@ -3944,13 +4031,13 @@
             <v>1d6 perforant</v>
           </cell>
           <cell r="D36" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E36" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F36" t="str">
             <v>2 kg</v>
-          </cell>
-          <cell r="E36" t="str">
-            <v>5 po</v>
-          </cell>
-          <cell r="F36" t="str">
-            <v>Lancer (portée 6 m/18 m), polyvalente (1d8)</v>
           </cell>
         </row>
         <row r="37">
@@ -3969,13 +4056,13 @@
             <v>1d6 perforant</v>
           </cell>
           <cell r="D38" t="str">
+            <v xml:space="preserve">1d6 </v>
+          </cell>
+          <cell r="E38" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F38" t="str">
             <v>1,5 kg</v>
-          </cell>
-          <cell r="E38" t="str">
-            <v>75 po</v>
-          </cell>
-          <cell r="F38" t="str">
-            <v>Munitions (portée 9 m/36 m), légère, chargement</v>
           </cell>
         </row>
         <row r="39">
@@ -3989,13 +4076,13 @@
             <v>1d10 perforant</v>
           </cell>
           <cell r="D39" t="str">
+            <v xml:space="preserve">1d10 </v>
+          </cell>
+          <cell r="E39" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F39" t="str">
             <v>9 kg</v>
-          </cell>
-          <cell r="E39" t="str">
-            <v>50 po</v>
-          </cell>
-          <cell r="F39" t="str">
-            <v>Munitions (portée 30 m/120 m), lourde, chargement, à deux mains</v>
           </cell>
         </row>
         <row r="40">
@@ -4009,13 +4096,13 @@
             <v>1d8 perforant</v>
           </cell>
           <cell r="D40" t="str">
+            <v xml:space="preserve">1d8 </v>
+          </cell>
+          <cell r="E40" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F40" t="str">
             <v>1 kg</v>
-          </cell>
-          <cell r="E40" t="str">
-            <v>50 po</v>
-          </cell>
-          <cell r="F40" t="str">
-            <v>Munitions (portée 45 m/180 m), lourde, à deux mains</v>
           </cell>
         </row>
         <row r="41">
@@ -4025,14 +4112,8 @@
           <cell r="B41" t="str">
             <v>Net</v>
           </cell>
-          <cell r="D41" t="str">
+          <cell r="F41" t="str">
             <v>1,5 kg</v>
-          </cell>
-          <cell r="E41" t="str">
-            <v>1 po</v>
-          </cell>
-          <cell r="F41" t="str">
-            <v>Spécial, lancer (portée 1,50 m/ 4,50 m)</v>
           </cell>
         </row>
         <row r="42">
@@ -4046,13 +4127,13 @@
             <v>1 perforant</v>
           </cell>
           <cell r="D42" t="str">
+            <v xml:space="preserve">1 </v>
+          </cell>
+          <cell r="E42" t="str">
+            <v>Perforant</v>
+          </cell>
+          <cell r="F42" t="str">
             <v>500 g</v>
-          </cell>
-          <cell r="E42" t="str">
-            <v>10 po</v>
-          </cell>
-          <cell r="F42" t="str">
-            <v>Munitions (portée 7,50 m/30 m), chargement</v>
           </cell>
         </row>
       </sheetData>
@@ -4067,6 +4148,7 @@
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4083,10 +4165,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C1:C11" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C1:C11" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="C1:C11"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Dés" dataDxfId="0"/>
+    <tableColumn id="1" name="Dés" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4393,7 +4475,7 @@
   <sheetViews>
     <sheetView showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="M5" activeCellId="1" sqref="H5:H10 M5:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4418,10 +4500,10 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="187" t="s">
+      <c r="C1" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="187"/>
+      <c r="D1" s="201"/>
       <c r="E1" s="93" t="s">
         <v>325</v>
       </c>
@@ -4434,10 +4516,10 @@
       <c r="H1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="192" t="s">
+      <c r="I1" s="183" t="s">
         <v>270</v>
       </c>
-      <c r="J1" s="192"/>
+      <c r="J1" s="183"/>
       <c r="K1" s="3"/>
       <c r="L1" s="79"/>
       <c r="M1" s="79"/>
@@ -4446,10 +4528,10 @@
       <c r="B2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="186" t="s">
+      <c r="C2" s="200" t="s">
         <v>301</v>
       </c>
-      <c r="D2" s="186"/>
+      <c r="D2" s="200"/>
       <c r="E2" s="22" t="s">
         <v>324</v>
       </c>
@@ -4463,37 +4545,37 @@
       <c r="H2" s="45">
         <v>0</v>
       </c>
-      <c r="I2" s="193">
+      <c r="I2" s="206">
         <f>VLOOKUP($G$2+1,[1]Niveaux!$A$2:$C$21,2)</f>
         <v>300</v>
       </c>
-      <c r="J2" s="193"/>
-      <c r="K2" s="206"/>
-      <c r="L2" s="206"/>
-      <c r="M2" s="207"/>
+      <c r="J2" s="206"/>
+      <c r="K2" s="161"/>
+      <c r="L2" s="161"/>
+      <c r="M2" s="162"/>
     </row>
     <row r="3" spans="2:15" ht="11.25" customHeight="1">
       <c r="K3" s="102"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
       <c r="E4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="189" t="s">
+      <c r="H4" s="203" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="189"/>
-      <c r="J4" s="189"/>
+      <c r="I4" s="203"/>
+      <c r="J4" s="203"/>
       <c r="K4" s="145"/>
-      <c r="L4" s="192" t="s">
+      <c r="L4" s="183" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="192"/>
+      <c r="M4" s="183"/>
     </row>
     <row r="5" spans="2:15">
       <c r="C5" s="2" t="s">
@@ -4620,10 +4702,10 @@
       </c>
     </row>
     <row r="10" spans="2:15">
-      <c r="C10" s="196" t="s">
+      <c r="C10" s="188" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="197"/>
+      <c r="D10" s="189"/>
       <c r="E10" s="64">
         <v>14</v>
       </c>
@@ -4666,10 +4748,10 @@
       <c r="L12" s="12"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="C13" s="196" t="s">
+      <c r="C13" s="188" t="s">
         <v>280</v>
       </c>
-      <c r="D13" s="197"/>
+      <c r="D13" s="189"/>
       <c r="E13" s="40"/>
       <c r="F13" s="10"/>
       <c r="G13" s="12"/>
@@ -4713,17 +4795,17 @@
         <v>25</v>
       </c>
       <c r="I16" s="14"/>
-      <c r="L16" s="218" t="s">
+      <c r="L16" s="180" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="218"/>
-      <c r="N16" s="218"/>
+      <c r="M16" s="180"/>
+      <c r="N16" s="180"/>
     </row>
     <row r="17" spans="3:14">
-      <c r="C17" s="190">
+      <c r="C17" s="204">
         <v>11</v>
       </c>
-      <c r="D17" s="191"/>
+      <c r="D17" s="205"/>
       <c r="E17" s="109"/>
       <c r="F17" s="110"/>
       <c r="G17" s="110"/>
@@ -4732,10 +4814,10 @@
       <c r="L17" s="38">
         <v>1</v>
       </c>
-      <c r="M17" s="219" t="s">
+      <c r="M17" s="181" t="s">
         <v>55</v>
       </c>
-      <c r="N17" s="168"/>
+      <c r="N17" s="182"/>
     </row>
     <row r="18" spans="3:14">
       <c r="C18" s="103" t="s">
@@ -4758,16 +4840,16 @@
       <c r="L18" s="39">
         <v>0</v>
       </c>
-      <c r="M18" s="168" t="s">
+      <c r="M18" s="182" t="s">
         <v>56</v>
       </c>
-      <c r="N18" s="168"/>
+      <c r="N18" s="182"/>
     </row>
     <row r="19" spans="3:14">
-      <c r="C19" s="194">
+      <c r="C19" s="186">
         <v>10</v>
       </c>
-      <c r="D19" s="195"/>
+      <c r="D19" s="187"/>
       <c r="E19" s="106">
         <v>10</v>
       </c>
@@ -4785,41 +4867,41 @@
       <c r="L19" s="39">
         <v>0</v>
       </c>
-      <c r="M19" s="168" t="s">
+      <c r="M19" s="182" t="s">
         <v>57</v>
       </c>
-      <c r="N19" s="168"/>
+      <c r="N19" s="182"/>
     </row>
     <row r="20" spans="3:14">
       <c r="C20" s="114" t="s">
         <v>327</v>
       </c>
       <c r="D20" s="115"/>
-      <c r="E20" s="203" t="s">
+      <c r="E20" s="197" t="s">
         <v>328</v>
       </c>
-      <c r="F20" s="203"/>
+      <c r="F20" s="197"/>
       <c r="G20" s="141" t="s">
         <v>365</v>
       </c>
       <c r="L20" s="39">
         <v>0</v>
       </c>
-      <c r="M20" s="168" t="s">
+      <c r="M20" s="182" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="168"/>
+      <c r="N20" s="182"/>
     </row>
     <row r="21" spans="3:14">
-      <c r="C21" s="194">
-        <v>0</v>
-      </c>
-      <c r="D21" s="195"/>
-      <c r="E21" s="200" t="str">
+      <c r="C21" s="186">
+        <v>0</v>
+      </c>
+      <c r="D21" s="187"/>
+      <c r="E21" s="194" t="str">
         <f>VLOOKUP($G$2,Classe!$A$3:$F$22,4)</f>
         <v>-</v>
       </c>
-      <c r="F21" s="200"/>
+      <c r="F21" s="194"/>
       <c r="G21" s="142" t="str">
         <f>VLOOKUP($G$2,Classe!A3:G22,7)</f>
         <v>-</v>
@@ -4827,10 +4909,10 @@
       <c r="L21" s="40">
         <v>0</v>
       </c>
-      <c r="M21" s="220" t="s">
+      <c r="M21" s="184" t="s">
         <v>59</v>
       </c>
-      <c r="N21" s="221"/>
+      <c r="N21" s="185"/>
     </row>
     <row r="22" spans="3:14">
       <c r="C22" s="116"/>
@@ -4842,20 +4924,20 @@
         <v>285</v>
       </c>
       <c r="D24" s="89"/>
-      <c r="E24" s="208" t="s">
+      <c r="E24" s="163" t="s">
         <v>261</v>
       </c>
-      <c r="F24" s="208"/>
-      <c r="G24" s="208"/>
+      <c r="F24" s="163"/>
+      <c r="G24" s="163"/>
       <c r="J24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K24" s="209" t="s">
+      <c r="K24" s="164" t="s">
         <v>64</v>
       </c>
-      <c r="L24" s="210"/>
-      <c r="M24" s="210"/>
-      <c r="N24" s="211"/>
+      <c r="L24" s="165"/>
+      <c r="M24" s="165"/>
+      <c r="N24" s="166"/>
     </row>
     <row r="25" spans="3:14">
       <c r="C25" s="155" t="s">
@@ -4864,16 +4946,16 @@
       <c r="D25" s="156" t="s">
         <v>362</v>
       </c>
-      <c r="E25" s="201"/>
-      <c r="F25" s="201"/>
-      <c r="G25" s="202"/>
+      <c r="E25" s="195"/>
+      <c r="F25" s="195"/>
+      <c r="G25" s="196"/>
       <c r="J25" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="K25" s="181"/>
-      <c r="L25" s="182"/>
-      <c r="M25" s="182"/>
-      <c r="N25" s="183"/>
+      <c r="K25" s="167"/>
+      <c r="L25" s="168"/>
+      <c r="M25" s="168"/>
+      <c r="N25" s="169"/>
     </row>
     <row r="26" spans="3:14" ht="14.25" customHeight="1">
       <c r="C26" s="157" t="s">
@@ -4882,21 +4964,21 @@
       <c r="D26" s="158" t="s">
         <v>361</v>
       </c>
-      <c r="E26" s="184" t="str">
+      <c r="E26" s="178" t="str">
         <f>VLOOKUP($G$2,Classe!A3:F22,3,FALSE)</f>
         <v>1d4</v>
       </c>
-      <c r="F26" s="184"/>
-      <c r="G26" s="185"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="179"/>
       <c r="J26" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="K26" s="179" t="str">
+      <c r="K26" s="170" t="str">
         <f>VLOOKUP($K24,[1]Armes!$A$2:$F$42,3)</f>
         <v>1d6 contondant</v>
       </c>
-      <c r="L26" s="180"/>
-      <c r="M26" s="180"/>
+      <c r="L26" s="171"/>
+      <c r="M26" s="171"/>
       <c r="N26" s="120">
         <f>IF(IFERROR(INDEX(Maitrise!$A$2:$B$40,MATCH($K$24,Maitrise!$B$2:$B$40,0),1),0)=1,Maitrise!$P$2,"")</f>
         <v>2</v>
@@ -4909,21 +4991,21 @@
       <c r="D27" s="158" t="s">
         <v>281</v>
       </c>
-      <c r="E27" s="184" t="s">
+      <c r="E27" s="178" t="s">
         <v>283</v>
       </c>
-      <c r="F27" s="184"/>
-      <c r="G27" s="185"/>
-      <c r="J27" s="169" t="s">
+      <c r="F27" s="178"/>
+      <c r="G27" s="179"/>
+      <c r="J27" s="207" t="s">
         <v>158</v>
       </c>
-      <c r="K27" s="212" t="str">
+      <c r="K27" s="172" t="str">
         <f>VLOOKUP($K24,[1]Armes!$A$2:$F$42,4,FALSE)&amp;" - "&amp;VLOOKUP($K24,[1]Armes!$A$2:$F$42,6,FALSE)</f>
-        <v>2 kg - Polyvalente (1d8)</v>
-      </c>
-      <c r="L27" s="213"/>
-      <c r="M27" s="213"/>
-      <c r="N27" s="214"/>
+        <v>1d6  - 2 kg</v>
+      </c>
+      <c r="L27" s="173"/>
+      <c r="M27" s="173"/>
+      <c r="N27" s="174"/>
     </row>
     <row r="28" spans="3:14">
       <c r="C28" s="159">
@@ -4932,81 +5014,81 @@
       <c r="D28" s="158" t="s">
         <v>282</v>
       </c>
-      <c r="E28" s="184" t="s">
+      <c r="E28" s="178" t="s">
         <v>326</v>
       </c>
-      <c r="F28" s="184"/>
-      <c r="G28" s="185"/>
-      <c r="J28" s="170"/>
-      <c r="K28" s="212"/>
-      <c r="L28" s="213"/>
-      <c r="M28" s="213"/>
-      <c r="N28" s="214"/>
+      <c r="F28" s="178"/>
+      <c r="G28" s="179"/>
+      <c r="J28" s="208"/>
+      <c r="K28" s="172"/>
+      <c r="L28" s="173"/>
+      <c r="M28" s="173"/>
+      <c r="N28" s="174"/>
     </row>
     <row r="29" spans="3:14">
       <c r="C29" s="39"/>
       <c r="D29" s="85"/>
-      <c r="E29" s="184"/>
-      <c r="F29" s="184"/>
-      <c r="G29" s="185"/>
-      <c r="J29" s="171"/>
-      <c r="K29" s="215"/>
-      <c r="L29" s="216"/>
-      <c r="M29" s="216"/>
-      <c r="N29" s="217"/>
+      <c r="E29" s="178"/>
+      <c r="F29" s="178"/>
+      <c r="G29" s="179"/>
+      <c r="J29" s="209"/>
+      <c r="K29" s="175"/>
+      <c r="L29" s="176"/>
+      <c r="M29" s="176"/>
+      <c r="N29" s="177"/>
     </row>
     <row r="30" spans="3:14">
       <c r="C30" s="39"/>
       <c r="D30" s="85"/>
-      <c r="E30" s="184"/>
-      <c r="F30" s="184"/>
-      <c r="G30" s="185"/>
+      <c r="E30" s="178"/>
+      <c r="F30" s="178"/>
+      <c r="G30" s="179"/>
     </row>
     <row r="31" spans="3:14">
       <c r="C31" s="39"/>
       <c r="D31" s="85"/>
-      <c r="E31" s="184"/>
-      <c r="F31" s="184"/>
-      <c r="G31" s="185"/>
+      <c r="E31" s="178"/>
+      <c r="F31" s="178"/>
+      <c r="G31" s="179"/>
       <c r="J31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K31" s="209" t="s">
+      <c r="K31" s="164" t="s">
         <v>330</v>
       </c>
-      <c r="L31" s="210"/>
-      <c r="M31" s="210"/>
-      <c r="N31" s="211"/>
+      <c r="L31" s="165"/>
+      <c r="M31" s="165"/>
+      <c r="N31" s="166"/>
     </row>
     <row r="32" spans="3:14">
       <c r="C32" s="39"/>
       <c r="D32" s="85"/>
-      <c r="E32" s="184"/>
-      <c r="F32" s="184"/>
-      <c r="G32" s="185"/>
+      <c r="E32" s="178"/>
+      <c r="F32" s="178"/>
+      <c r="G32" s="179"/>
       <c r="J32" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="K32" s="181"/>
-      <c r="L32" s="182"/>
-      <c r="M32" s="182"/>
-      <c r="N32" s="183"/>
+      <c r="K32" s="167"/>
+      <c r="L32" s="168"/>
+      <c r="M32" s="168"/>
+      <c r="N32" s="169"/>
     </row>
     <row r="33" spans="3:14" ht="15" customHeight="1">
       <c r="C33" s="39"/>
       <c r="D33" s="85"/>
-      <c r="E33" s="184"/>
-      <c r="F33" s="184"/>
-      <c r="G33" s="185"/>
+      <c r="E33" s="178"/>
+      <c r="F33" s="178"/>
+      <c r="G33" s="179"/>
       <c r="J33" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="K33" s="179" t="str">
+      <c r="K33" s="170" t="str">
         <f>VLOOKUP($K31,[1]Armes!$A$2:$F$42,3)</f>
         <v>1d4 tranchant</v>
       </c>
-      <c r="L33" s="180"/>
-      <c r="M33" s="180"/>
+      <c r="L33" s="171"/>
+      <c r="M33" s="171"/>
       <c r="N33" s="120">
         <f>IF(IFERROR(INDEX(Maitrise!$A$2:$B$40,MATCH($K$31,Maitrise!$B$2:$B$40,0),1),0)=1,Maitrise!$P$2,"")</f>
         <v>2</v>
@@ -5015,54 +5097,54 @@
     <row r="34" spans="3:14" ht="16.5" customHeight="1">
       <c r="C34" s="39"/>
       <c r="D34" s="85"/>
-      <c r="E34" s="184"/>
-      <c r="F34" s="184"/>
-      <c r="G34" s="185"/>
+      <c r="E34" s="178"/>
+      <c r="F34" s="178"/>
+      <c r="G34" s="179"/>
       <c r="J34" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="K34" s="178">
+      <c r="K34" s="216">
         <v>10</v>
       </c>
-      <c r="L34" s="163"/>
-      <c r="M34" s="163"/>
-      <c r="N34" s="164"/>
+      <c r="L34" s="192"/>
+      <c r="M34" s="192"/>
+      <c r="N34" s="193"/>
     </row>
     <row r="35" spans="3:14" ht="15" customHeight="1">
       <c r="C35" s="39"/>
       <c r="D35" s="85"/>
-      <c r="E35" s="184"/>
-      <c r="F35" s="184"/>
-      <c r="G35" s="185"/>
-      <c r="J35" s="169" t="s">
+      <c r="E35" s="178"/>
+      <c r="F35" s="178"/>
+      <c r="G35" s="179"/>
+      <c r="J35" s="207" t="s">
         <v>158</v>
       </c>
-      <c r="K35" s="172" t="str">
+      <c r="K35" s="210" t="str">
         <f>VLOOKUP($K31,[1]Armes!$A$2:$F$42,4,FALSE)&amp;" - "&amp;VLOOKUP($K31,[1]Armes!$A$2:$F$42,6,FALSE)</f>
-        <v>0 g - Munitions (portée 9 m/36 m)</v>
-      </c>
-      <c r="L35" s="173"/>
-      <c r="M35" s="173"/>
-      <c r="N35" s="174"/>
+        <v>1d4  - 0 g</v>
+      </c>
+      <c r="L35" s="211"/>
+      <c r="M35" s="211"/>
+      <c r="N35" s="212"/>
     </row>
     <row r="36" spans="3:14">
       <c r="C36" s="40"/>
       <c r="D36" s="83"/>
-      <c r="E36" s="204"/>
-      <c r="F36" s="204"/>
-      <c r="G36" s="205"/>
-      <c r="J36" s="170"/>
-      <c r="K36" s="172"/>
-      <c r="L36" s="173"/>
-      <c r="M36" s="173"/>
-      <c r="N36" s="174"/>
+      <c r="E36" s="198"/>
+      <c r="F36" s="198"/>
+      <c r="G36" s="199"/>
+      <c r="J36" s="208"/>
+      <c r="K36" s="210"/>
+      <c r="L36" s="211"/>
+      <c r="M36" s="211"/>
+      <c r="N36" s="212"/>
     </row>
     <row r="37" spans="3:14">
-      <c r="J37" s="171"/>
-      <c r="K37" s="175"/>
-      <c r="L37" s="176"/>
-      <c r="M37" s="176"/>
-      <c r="N37" s="177"/>
+      <c r="J37" s="209"/>
+      <c r="K37" s="213"/>
+      <c r="L37" s="214"/>
+      <c r="M37" s="214"/>
+      <c r="N37" s="215"/>
     </row>
     <row r="38" spans="3:14">
       <c r="C38" s="95" t="s">
@@ -5081,121 +5163,121 @@
       <c r="D39" s="96">
         <v>0</v>
       </c>
-      <c r="E39" s="198"/>
-      <c r="F39" s="198"/>
-      <c r="G39" s="199"/>
+      <c r="E39" s="190"/>
+      <c r="F39" s="190"/>
+      <c r="G39" s="191"/>
       <c r="J39" s="154"/>
-      <c r="K39" s="165"/>
-      <c r="L39" s="165"/>
-      <c r="M39" s="165"/>
-      <c r="N39" s="165"/>
+      <c r="K39" s="219"/>
+      <c r="L39" s="219"/>
+      <c r="M39" s="219"/>
+      <c r="N39" s="219"/>
     </row>
     <row r="40" spans="3:14">
       <c r="C40" s="99"/>
       <c r="D40" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="E40" s="163"/>
-      <c r="F40" s="163"/>
-      <c r="G40" s="164"/>
+      <c r="E40" s="192"/>
+      <c r="F40" s="192"/>
+      <c r="G40" s="193"/>
       <c r="J40" s="154"/>
-      <c r="K40" s="167"/>
-      <c r="L40" s="167"/>
-      <c r="M40" s="167"/>
-      <c r="N40" s="167"/>
+      <c r="K40" s="221"/>
+      <c r="L40" s="221"/>
+      <c r="M40" s="221"/>
+      <c r="N40" s="221"/>
     </row>
     <row r="41" spans="3:14">
       <c r="C41" s="99"/>
       <c r="D41" s="97" t="s">
         <v>161</v>
       </c>
-      <c r="E41" s="163"/>
-      <c r="F41" s="163"/>
-      <c r="G41" s="164"/>
+      <c r="E41" s="192"/>
+      <c r="F41" s="192"/>
+      <c r="G41" s="193"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="154"/>
-      <c r="K41" s="166"/>
-      <c r="L41" s="166"/>
-      <c r="M41" s="166"/>
-      <c r="N41" s="166"/>
+      <c r="K41" s="220"/>
+      <c r="L41" s="220"/>
+      <c r="M41" s="220"/>
+      <c r="N41" s="220"/>
     </row>
     <row r="42" spans="3:14">
       <c r="C42" s="99"/>
       <c r="D42" s="97" t="s">
         <v>166</v>
       </c>
-      <c r="E42" s="163"/>
-      <c r="F42" s="163"/>
-      <c r="G42" s="164"/>
+      <c r="E42" s="192"/>
+      <c r="F42" s="192"/>
+      <c r="G42" s="193"/>
     </row>
     <row r="43" spans="3:14">
       <c r="C43" s="99"/>
       <c r="D43" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="E43" s="163"/>
-      <c r="F43" s="163"/>
-      <c r="G43" s="164"/>
+      <c r="E43" s="192"/>
+      <c r="F43" s="192"/>
+      <c r="G43" s="193"/>
     </row>
     <row r="44" spans="3:14">
       <c r="C44" s="99"/>
       <c r="D44" s="97" t="s">
         <v>167</v>
       </c>
-      <c r="E44" s="163"/>
-      <c r="F44" s="163"/>
-      <c r="G44" s="164"/>
+      <c r="E44" s="192"/>
+      <c r="F44" s="192"/>
+      <c r="G44" s="193"/>
     </row>
     <row r="45" spans="3:14">
       <c r="C45" s="99"/>
       <c r="D45" s="97" t="s">
         <v>164</v>
       </c>
-      <c r="E45" s="163"/>
-      <c r="F45" s="163"/>
-      <c r="G45" s="164"/>
+      <c r="E45" s="192"/>
+      <c r="F45" s="192"/>
+      <c r="G45" s="193"/>
     </row>
     <row r="46" spans="3:14">
       <c r="C46" s="100"/>
       <c r="D46" s="97" t="s">
         <v>168</v>
       </c>
-      <c r="E46" s="163"/>
-      <c r="F46" s="163"/>
-      <c r="G46" s="164"/>
+      <c r="E46" s="192"/>
+      <c r="F46" s="192"/>
+      <c r="G46" s="193"/>
     </row>
     <row r="47" spans="3:14">
       <c r="C47" s="99"/>
       <c r="D47" s="97" t="s">
         <v>165</v>
       </c>
-      <c r="E47" s="163"/>
-      <c r="F47" s="163"/>
-      <c r="G47" s="164"/>
+      <c r="E47" s="192"/>
+      <c r="F47" s="192"/>
+      <c r="G47" s="193"/>
     </row>
     <row r="48" spans="3:14">
       <c r="C48" s="99"/>
       <c r="D48" s="97" t="s">
         <v>169</v>
       </c>
-      <c r="E48" s="163"/>
-      <c r="F48" s="163"/>
-      <c r="G48" s="164"/>
+      <c r="E48" s="192"/>
+      <c r="F48" s="192"/>
+      <c r="G48" s="193"/>
     </row>
     <row r="49" spans="3:15">
       <c r="C49" s="99"/>
       <c r="D49" s="147"/>
-      <c r="E49" s="163"/>
-      <c r="F49" s="163"/>
-      <c r="G49" s="164"/>
+      <c r="E49" s="192"/>
+      <c r="F49" s="192"/>
+      <c r="G49" s="193"/>
     </row>
     <row r="50" spans="3:15">
       <c r="C50" s="101"/>
       <c r="D50" s="160"/>
-      <c r="E50" s="161"/>
-      <c r="F50" s="161"/>
-      <c r="G50" s="162"/>
+      <c r="E50" s="217"/>
+      <c r="F50" s="217"/>
+      <c r="G50" s="218"/>
     </row>
     <row r="56" spans="3:15">
       <c r="I56" s="146"/>
@@ -5282,6 +5364,50 @@
   </sheetData>
   <sheetProtection sheet="1" scenarios="1"/>
   <mergeCells count="60">
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="K35:N37"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="K24:N24"/>
@@ -5298,53 +5424,9 @@
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:G28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="K35:N37"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="J35:J37"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="K39:N39"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:I10">
-    <cfRule type="expression" dxfId="9" priority="27">
+    <cfRule type="expression" dxfId="5" priority="27">
       <formula>$J5=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5377,12 +5459,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5:M10 M17:M21">
-    <cfRule type="expression" dxfId="8" priority="39">
+    <cfRule type="expression" dxfId="4" priority="39">
       <formula>$L5=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I2">
-    <cfRule type="expression" dxfId="7" priority="40">
+    <cfRule type="expression" dxfId="3" priority="40">
       <formula>$H$2&gt;=$I$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5401,7 +5483,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:E36">
-    <cfRule type="expression" dxfId="6" priority="45">
+    <cfRule type="expression" dxfId="2" priority="45">
       <formula>$C25=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6576,7 +6658,7 @@
     <mergeCell ref="D5:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="N2:N19 E6:E10 B13:B29 B2:B11 B31:B34 B36:B40 E2:E4 E12:E15 E17:E19 L2:L19 J2:J19 H2:H19">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>A2=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6676,9 +6758,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showRowColHeaders="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7970,7 +8052,9 @@
         <v>251</v>
       </c>
       <c r="D65" t="str">
-        <f t="shared" si="0"/>
+        <f>""""&amp;B65&amp;""": {  ""Caracteristic"": """&amp;LEFT(RIGHT(C65,4),3)&amp;""",
+  ""Name"": """&amp;B65&amp;"""
+ }"</f>
         <v>"Pêche": {  "Caracteristic": "SAG",
   "Name": "Pêche"
  }</v>
@@ -8630,7 +8714,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:C81">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A2=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8736,10 +8820,10 @@
       <c r="F2" s="43">
         <v>0</v>
       </c>
-      <c r="H2" s="233"/>
-      <c r="I2" s="234"/>
-      <c r="J2" s="234"/>
-      <c r="K2" s="235"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="229"/>
+      <c r="J2" s="229"/>
+      <c r="K2" s="230"/>
       <c r="L2" s="67">
         <v>0</v>
       </c>
@@ -8751,245 +8835,275 @@
       <c r="A3" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="230" t="s">
+      <c r="B3" s="233" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="230"/>
-      <c r="D3" s="230"/>
-      <c r="E3" s="230"/>
-      <c r="F3" s="231"/>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="234"/>
       <c r="H3" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="I3" s="232" t="s">
+      <c r="I3" s="235" t="s">
         <v>261</v>
       </c>
-      <c r="J3" s="232"/>
+      <c r="J3" s="235"/>
       <c r="K3" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="230" t="s">
+      <c r="L3" s="233" t="s">
         <v>261</v>
       </c>
-      <c r="M3" s="231"/>
+      <c r="M3" s="234"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="39"/>
-      <c r="B4" s="226"/>
-      <c r="C4" s="226"/>
-      <c r="D4" s="226"/>
-      <c r="E4" s="226"/>
-      <c r="F4" s="227"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="231"/>
+      <c r="D4" s="231"/>
+      <c r="E4" s="231"/>
+      <c r="F4" s="232"/>
       <c r="H4" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="I4" s="226"/>
-      <c r="J4" s="227"/>
+      <c r="I4" s="231"/>
+      <c r="J4" s="232"/>
       <c r="K4" s="39"/>
-      <c r="L4" s="226"/>
-      <c r="M4" s="227"/>
+      <c r="L4" s="231"/>
+      <c r="M4" s="232"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="39"/>
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="227"/>
+      <c r="B5" s="231"/>
+      <c r="C5" s="231"/>
+      <c r="D5" s="231"/>
+      <c r="E5" s="231"/>
+      <c r="F5" s="232"/>
       <c r="H5" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="I5" s="226"/>
-      <c r="J5" s="227"/>
+      <c r="I5" s="231"/>
+      <c r="J5" s="232"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="226"/>
-      <c r="M5" s="227"/>
+      <c r="L5" s="231"/>
+      <c r="M5" s="232"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="39"/>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="227"/>
+      <c r="B6" s="231"/>
+      <c r="C6" s="231"/>
+      <c r="D6" s="231"/>
+      <c r="E6" s="231"/>
+      <c r="F6" s="232"/>
       <c r="H6" s="39"/>
-      <c r="I6" s="226"/>
-      <c r="J6" s="227"/>
+      <c r="I6" s="231"/>
+      <c r="J6" s="232"/>
       <c r="K6" s="39"/>
-      <c r="L6" s="226"/>
-      <c r="M6" s="227"/>
+      <c r="L6" s="231"/>
+      <c r="M6" s="232"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="39"/>
-      <c r="B7" s="226"/>
-      <c r="C7" s="226"/>
-      <c r="D7" s="226"/>
-      <c r="E7" s="226"/>
-      <c r="F7" s="227"/>
+      <c r="B7" s="231"/>
+      <c r="C7" s="231"/>
+      <c r="D7" s="231"/>
+      <c r="E7" s="231"/>
+      <c r="F7" s="232"/>
       <c r="H7" s="39"/>
-      <c r="I7" s="226"/>
-      <c r="J7" s="227"/>
+      <c r="I7" s="231"/>
+      <c r="J7" s="232"/>
       <c r="K7" s="39"/>
-      <c r="L7" s="226"/>
-      <c r="M7" s="227"/>
+      <c r="L7" s="231"/>
+      <c r="M7" s="232"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="39"/>
-      <c r="B8" s="226"/>
-      <c r="C8" s="226"/>
-      <c r="D8" s="226"/>
-      <c r="E8" s="226"/>
-      <c r="F8" s="227"/>
+      <c r="B8" s="231"/>
+      <c r="C8" s="231"/>
+      <c r="D8" s="231"/>
+      <c r="E8" s="231"/>
+      <c r="F8" s="232"/>
       <c r="H8" s="39"/>
-      <c r="I8" s="226"/>
-      <c r="J8" s="227"/>
+      <c r="I8" s="231"/>
+      <c r="J8" s="232"/>
       <c r="K8" s="75" t="s">
         <v>267</v>
       </c>
-      <c r="L8" s="230" t="s">
+      <c r="L8" s="233" t="s">
         <v>261</v>
       </c>
-      <c r="M8" s="231"/>
+      <c r="M8" s="234"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="39"/>
-      <c r="B9" s="226"/>
-      <c r="C9" s="226"/>
-      <c r="D9" s="226"/>
-      <c r="E9" s="226"/>
-      <c r="F9" s="227"/>
+      <c r="B9" s="231"/>
+      <c r="C9" s="231"/>
+      <c r="D9" s="231"/>
+      <c r="E9" s="231"/>
+      <c r="F9" s="232"/>
       <c r="H9" s="39"/>
-      <c r="I9" s="226"/>
-      <c r="J9" s="227"/>
+      <c r="I9" s="231"/>
+      <c r="J9" s="232"/>
       <c r="K9" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="L9" s="226"/>
-      <c r="M9" s="227"/>
+      <c r="L9" s="231"/>
+      <c r="M9" s="232"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="39"/>
-      <c r="B10" s="226"/>
-      <c r="C10" s="226"/>
-      <c r="D10" s="226"/>
-      <c r="E10" s="226"/>
-      <c r="F10" s="227"/>
+      <c r="B10" s="231"/>
+      <c r="C10" s="231"/>
+      <c r="D10" s="231"/>
+      <c r="E10" s="231"/>
+      <c r="F10" s="232"/>
       <c r="H10" s="39"/>
-      <c r="I10" s="226"/>
-      <c r="J10" s="227"/>
+      <c r="I10" s="231"/>
+      <c r="J10" s="232"/>
       <c r="K10" s="39"/>
-      <c r="L10" s="226"/>
-      <c r="M10" s="227"/>
+      <c r="L10" s="231"/>
+      <c r="M10" s="232"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="39"/>
-      <c r="B11" s="226"/>
-      <c r="C11" s="226"/>
-      <c r="D11" s="226"/>
-      <c r="E11" s="226"/>
-      <c r="F11" s="227"/>
+      <c r="B11" s="231"/>
+      <c r="C11" s="231"/>
+      <c r="D11" s="231"/>
+      <c r="E11" s="231"/>
+      <c r="F11" s="232"/>
       <c r="H11" s="39"/>
-      <c r="I11" s="226"/>
-      <c r="J11" s="227"/>
+      <c r="I11" s="231"/>
+      <c r="J11" s="232"/>
       <c r="K11" s="39"/>
-      <c r="L11" s="226"/>
-      <c r="M11" s="227"/>
+      <c r="L11" s="231"/>
+      <c r="M11" s="232"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="39"/>
-      <c r="B12" s="226"/>
-      <c r="C12" s="226"/>
-      <c r="D12" s="226"/>
-      <c r="E12" s="226"/>
-      <c r="F12" s="227"/>
+      <c r="B12" s="231"/>
+      <c r="C12" s="231"/>
+      <c r="D12" s="231"/>
+      <c r="E12" s="231"/>
+      <c r="F12" s="232"/>
       <c r="H12" s="39"/>
-      <c r="I12" s="226"/>
-      <c r="J12" s="227"/>
+      <c r="I12" s="231"/>
+      <c r="J12" s="232"/>
       <c r="K12" s="39"/>
-      <c r="L12" s="226"/>
-      <c r="M12" s="227"/>
+      <c r="L12" s="231"/>
+      <c r="M12" s="232"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="39"/>
-      <c r="B13" s="226"/>
-      <c r="C13" s="226"/>
-      <c r="D13" s="226"/>
-      <c r="E13" s="226"/>
-      <c r="F13" s="227"/>
+      <c r="B13" s="231"/>
+      <c r="C13" s="231"/>
+      <c r="D13" s="231"/>
+      <c r="E13" s="231"/>
+      <c r="F13" s="232"/>
       <c r="H13" s="39"/>
-      <c r="I13" s="226"/>
-      <c r="J13" s="227"/>
+      <c r="I13" s="231"/>
+      <c r="J13" s="232"/>
       <c r="K13" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="L13" s="230" t="s">
+      <c r="L13" s="233" t="s">
         <v>261</v>
       </c>
-      <c r="M13" s="231"/>
+      <c r="M13" s="234"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="39"/>
-      <c r="B14" s="226"/>
-      <c r="C14" s="226"/>
-      <c r="D14" s="226"/>
-      <c r="E14" s="226"/>
-      <c r="F14" s="227"/>
+      <c r="B14" s="231"/>
+      <c r="C14" s="231"/>
+      <c r="D14" s="231"/>
+      <c r="E14" s="231"/>
+      <c r="F14" s="232"/>
       <c r="H14" s="39"/>
-      <c r="I14" s="226"/>
-      <c r="J14" s="227"/>
+      <c r="I14" s="231"/>
+      <c r="J14" s="232"/>
       <c r="K14" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="L14" s="226"/>
-      <c r="M14" s="227"/>
+      <c r="L14" s="231"/>
+      <c r="M14" s="232"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="39"/>
-      <c r="B15" s="226"/>
-      <c r="C15" s="226"/>
-      <c r="D15" s="226"/>
-      <c r="E15" s="226"/>
-      <c r="F15" s="227"/>
+      <c r="B15" s="231"/>
+      <c r="C15" s="231"/>
+      <c r="D15" s="231"/>
+      <c r="E15" s="231"/>
+      <c r="F15" s="232"/>
       <c r="H15" s="39"/>
-      <c r="I15" s="226"/>
-      <c r="J15" s="227"/>
+      <c r="I15" s="231"/>
+      <c r="J15" s="232"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="226"/>
-      <c r="M15" s="227"/>
+      <c r="L15" s="231"/>
+      <c r="M15" s="232"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="39"/>
-      <c r="B16" s="226"/>
-      <c r="C16" s="226"/>
-      <c r="D16" s="226"/>
-      <c r="E16" s="226"/>
-      <c r="F16" s="227"/>
+      <c r="B16" s="231"/>
+      <c r="C16" s="231"/>
+      <c r="D16" s="231"/>
+      <c r="E16" s="231"/>
+      <c r="F16" s="232"/>
       <c r="H16" s="39"/>
-      <c r="I16" s="226"/>
-      <c r="J16" s="227"/>
+      <c r="I16" s="231"/>
+      <c r="J16" s="232"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="226"/>
-      <c r="M16" s="227"/>
+      <c r="L16" s="231"/>
+      <c r="M16" s="232"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="40"/>
-      <c r="B17" s="228"/>
-      <c r="C17" s="228"/>
-      <c r="D17" s="228"/>
-      <c r="E17" s="228"/>
-      <c r="F17" s="229"/>
+      <c r="B17" s="226"/>
+      <c r="C17" s="226"/>
+      <c r="D17" s="226"/>
+      <c r="E17" s="226"/>
+      <c r="F17" s="227"/>
       <c r="H17" s="40" t="s">
         <v>265</v>
       </c>
-      <c r="I17" s="228"/>
-      <c r="J17" s="229"/>
+      <c r="I17" s="226"/>
+      <c r="J17" s="227"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="228"/>
-      <c r="M17" s="229"/>
+      <c r="L17" s="226"/>
+      <c r="M17" s="227"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="46">
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="L11:M11"/>
@@ -9006,36 +9120,6 @@
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B16:F16"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
@@ -9622,10 +9706,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="C1:D1048576"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9635,117 +9719,349 @@
     <col min="4" max="4" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>297</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1">
+      <c r="E1" s="236" t="s">
+        <v>367</v>
+      </c>
+      <c r="F1" s="236" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>311</v>
       </c>
       <c r="C2" s="91" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F2" t="s">
+        <v>380</v>
+      </c>
+      <c r="H2" t="str">
+        <f>""""&amp;E2&amp;""": {
+  ""Code"": """&amp;E2&amp;""",
+  ""Name"": """&amp;F2&amp;"""
+ }"</f>
+        <v>"Alcoholic": {
+  "Code": "Alcoholic",
+  "Name": "Alcoolisé"
+ }</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>310</v>
       </c>
       <c r="C3" s="91" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3" t="s">
+        <v>370</v>
+      </c>
+      <c r="F3" t="s">
+        <v>381</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H13" si="0">""""&amp;E3&amp;""": {
+  ""Code"": """&amp;E3&amp;""",
+  ""Name"": """&amp;F3&amp;"""
+ }"</f>
+        <v>"Bewitched": {
+  "Code": "Bewitched",
+  "Name": "Envouté"
+ }</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>309</v>
       </c>
       <c r="C4" s="91" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4" t="s">
+        <v>371</v>
+      </c>
+      <c r="F4" t="s">
+        <v>382</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>"Scared": {
+  "Code": "Scared",
+  "Name": "Effrayé"
+ }</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>308</v>
       </c>
       <c r="C5" s="91" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5" t="s">
+        <v>372</v>
+      </c>
+      <c r="F5" t="s">
+        <v>383</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>"Provocated": {
+  "Code": "Provocated",
+  "Name": "Provoqué"
+ }</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>307</v>
       </c>
       <c r="C6" s="91" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="E6" t="s">
+        <v>373</v>
+      </c>
+      <c r="F6" t="s">
+        <v>384</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>"Seduced": {
+  "Code": "Seduced",
+  "Name": "Séduit"
+ }</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>306</v>
       </c>
       <c r="C7" s="91" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="E7" t="s">
+        <v>374</v>
+      </c>
+      <c r="F7" t="s">
+        <v>385</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>"Stressed": {
+  "Code": "Stressed",
+  "Name": "Stressé"
+ }</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>305</v>
       </c>
       <c r="C8" s="91" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="E8" t="s">
+        <v>375</v>
+      </c>
+      <c r="F8" t="s">
+        <v>390</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>"Acidified": {
+  "Code": "Acidified",
+  "Name": "Acidifié"
+ }</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>304</v>
       </c>
       <c r="C9" s="91" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="E9" t="s">
+        <v>376</v>
+      </c>
+      <c r="F9" t="s">
+        <v>386</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Burned": {
+  "Code": "Burned",
+  "Name": "Brûlé"
+ }</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>299</v>
       </c>
       <c r="C10" s="91" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="E10" t="s">
+        <v>377</v>
+      </c>
+      <c r="F10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Electrified": {
+  "Code": "Electrified",
+  "Name": "Foudroyé"
+ }</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>300</v>
       </c>
       <c r="C11" s="92" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E11" t="s">
+        <v>378</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>"Cold": {
+  "Code": "Cold",
+  "Name": "Froid"
+ }</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1">
+      <c r="E12" t="s">
+        <v>379</v>
+      </c>
+      <c r="F12" t="s">
+        <v>388</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>"Drug": {
+  "Code": "Drug",
+  "Name": "Drogué"
+ }</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="E13" t="s">
+        <v>368</v>
+      </c>
+      <c r="F13" t="s">
+        <v>389</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>"Poisonned": {
+  "Code": "Poisonned",
+  "Name": "Empoisonné"
+ }</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>303</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="H15" t="str">
+        <f>CONCATENATE(H2,",
+",H3,",
+",H4,",
+",H5,",
+",H6,",
+",H7,",
+",H8,",
+",H9,",
+",H10,",
+",H11,",
+",H12,",
+",H13)</f>
+        <v>"Alcoholic": {
+  "Code": "Alcoholic",
+  "Name": "Alcoolisé"
+ },
+"Bewitched": {
+  "Code": "Bewitched",
+  "Name": "Envouté"
+ },
+"Scared": {
+  "Code": "Scared",
+  "Name": "Effrayé"
+ },
+"Provocated": {
+  "Code": "Provocated",
+  "Name": "Provoqué"
+ },
+"Seduced": {
+  "Code": "Seduced",
+  "Name": "Séduit"
+ },
+"Stressed": {
+  "Code": "Stressed",
+  "Name": "Stressé"
+ },
+"Acidified": {
+  "Code": "Acidified",
+  "Name": "Acidifié"
+ },
+"Burned": {
+  "Code": "Burned",
+  "Name": "Brûlé"
+ },
+"Electrified": {
+  "Code": "Electrified",
+  "Name": "Foudroyé"
+ },
+"Cold": {
+  "Code": "Cold",
+  "Name": "Froid"
+ },
+"Drug": {
+  "Code": "Drug",
+  "Name": "Drogué"
+ },
+"Poisonned": {
+  "Code": "Poisonned",
+  "Name": "Empoisonné"
+ }</v>
       </c>
     </row>
     <row r="18" ht="15" customHeight="1"/>
     <row r="37" ht="15" customHeight="1"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Capacities complement + Spells for specialisations + Bonus spells number + Fight style init
</commit_message>
<xml_diff>
--- a/Personnage.xlsx
+++ b/Personnage.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B7D850-B67F-4D57-9F98-D3253EB5E018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,17 @@
   <externalReferences>
     <externalReference r:id="rId8"/>
   </externalReferences>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1237,7 +1248,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
     <numFmt numFmtId="164" formatCode="&quot;D&quot;0"/>
     <numFmt numFmtId="165" formatCode="General&quot;m&quot;"/>
@@ -1996,101 +2007,71 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2107,6 +2088,14 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="171" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2123,146 +2112,110 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor auto="1"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2323,6 +2276,64 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor auto="1"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
@@ -2358,7 +2369,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2396,7 +2413,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="15" name="Groupe 14"/>
+        <xdr:cNvPr id="15" name="Groupe 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -2409,7 +2432,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="3" name="Image 2"/>
+          <xdr:cNvPr id="3" name="Image 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2444,7 +2473,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="" fLocksText="0">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Hexagone 3"/>
+          <xdr:cNvPr id="4" name="Hexagone 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2487,7 +2522,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="" fLocksText="0">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Hexagone 4"/>
+          <xdr:cNvPr id="5" name="Hexagone 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2530,7 +2571,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="" fLocksText="0">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Hexagone 5"/>
+          <xdr:cNvPr id="6" name="Hexagone 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2573,7 +2620,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Hexagone 7"/>
+          <xdr:cNvPr id="8" name="Hexagone 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2616,7 +2669,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="" fLocksText="0">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="Hexagone 8"/>
+          <xdr:cNvPr id="9" name="Hexagone 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2659,7 +2718,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="" fLocksText="0">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="Hexagone 9"/>
+          <xdr:cNvPr id="10" name="Hexagone 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2702,7 +2767,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="" fLocksText="0">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="Hexagone 10"/>
+          <xdr:cNvPr id="11" name="Hexagone 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2745,7 +2816,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="" fLocksText="0">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="Hexagone 11"/>
+          <xdr:cNvPr id="12" name="Hexagone 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2788,7 +2865,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="" fLocksText="0">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="Hexagone 12"/>
+          <xdr:cNvPr id="13" name="Hexagone 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2831,7 +2914,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="" fLocksText="0">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="Hexagone 13"/>
+          <xdr:cNvPr id="14" name="Hexagone 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2890,7 +2979,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Image 23"/>
+        <xdr:cNvPr id="24" name="Image 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2933,7 +3028,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2971,7 +3072,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 3"/>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3011,7 +3118,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 4"/>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3058,6 +3171,7 @@
       <sheetName val="Sous-races"/>
       <sheetName val="Classes"/>
       <sheetName val="Capacities"/>
+      <sheetName val="Specialisation-capacities"/>
       <sheetName val="Historiques"/>
       <sheetName val="Armes"/>
       <sheetName val="Armures"/>
@@ -3304,11 +3418,17 @@
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
-      <sheetData sheetId="6">
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7">
         <row r="2">
           <cell r="A2" t="str">
             <v>Armes courantes de corps à corps</v>
           </cell>
+          <cell r="B2"/>
+          <cell r="C2"/>
+          <cell r="D2"/>
+          <cell r="E2"/>
+          <cell r="F2"/>
         </row>
         <row r="3">
           <cell r="A3" t="str">
@@ -3514,6 +3634,11 @@
           <cell r="A13" t="str">
             <v>Armes courantes à distance</v>
           </cell>
+          <cell r="B13"/>
+          <cell r="C13"/>
+          <cell r="D13"/>
+          <cell r="E13"/>
+          <cell r="F13"/>
         </row>
         <row r="14">
           <cell r="A14" t="str">
@@ -3599,6 +3724,11 @@
           <cell r="A18" t="str">
             <v>Armes de guerre de corps à corps</v>
           </cell>
+          <cell r="B18"/>
+          <cell r="C18"/>
+          <cell r="D18"/>
+          <cell r="E18"/>
+          <cell r="F18"/>
         </row>
         <row r="19">
           <cell r="A19" t="str">
@@ -3964,6 +4094,11 @@
           <cell r="A37" t="str">
             <v>Armes de guerre à distance</v>
           </cell>
+          <cell r="B37"/>
+          <cell r="C37"/>
+          <cell r="D37"/>
+          <cell r="E37"/>
+          <cell r="F37"/>
         </row>
         <row r="38">
           <cell r="A38" t="str">
@@ -4032,6 +4167,9 @@
           <cell r="B41" t="str">
             <v>Net</v>
           </cell>
+          <cell r="C41"/>
+          <cell r="D41"/>
+          <cell r="E41"/>
           <cell r="F41" t="str">
             <v>1,5 kg</v>
           </cell>
@@ -4057,7 +4195,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
@@ -4072,36 +4209,37 @@
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="I1:I13" totalsRowShown="0">
-  <autoFilter ref="I1:I13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau3" displayName="Tableau3" ref="I1:I13" totalsRowShown="0">
+  <autoFilter ref="I1:I13" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Classes"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Classes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="C1:C11" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="C1:C11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau1" displayName="Tableau1" ref="C1:C11" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="C1:C11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Dés" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Dés" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:A14" totalsRowShown="0">
-  <autoFilter ref="A1:A14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="A1:A14" totalsRowShown="0">
+  <autoFilter ref="A1:A14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Races"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Races"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4183,6 +4321,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4218,6 +4373,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4393,7 +4565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O73"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -4423,10 +4595,10 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="187" t="s">
+      <c r="C1" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="187"/>
+      <c r="D1" s="202"/>
       <c r="E1" s="93" t="s">
         <v>325</v>
       </c>
@@ -4439,10 +4611,10 @@
       <c r="H1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="192" t="s">
+      <c r="I1" s="184" t="s">
         <v>270</v>
       </c>
-      <c r="J1" s="192"/>
+      <c r="J1" s="184"/>
       <c r="K1" s="3"/>
       <c r="L1" s="79"/>
       <c r="M1" s="79"/>
@@ -4451,54 +4623,54 @@
       <c r="B2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="186" t="s">
+      <c r="C2" s="201" t="s">
         <v>301</v>
       </c>
-      <c r="D2" s="186"/>
+      <c r="D2" s="201"/>
       <c r="E2" s="22" t="s">
         <v>324</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="G2" s="44">
+      <c r="G2" s="44" t="e">
         <f>COUNTIFS([1]Niveaux!$B$2:$B$21,"&lt;="&amp;H2)</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H2" s="45">
         <v>0</v>
       </c>
-      <c r="I2" s="193">
+      <c r="I2" s="207" t="e">
         <f>VLOOKUP($G$2+1,[1]Niveaux!$A$2:$C$21,2)</f>
-        <v>300</v>
-      </c>
-      <c r="J2" s="193"/>
-      <c r="K2" s="206"/>
-      <c r="L2" s="206"/>
-      <c r="M2" s="207"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J2" s="207"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="162"/>
+      <c r="M2" s="163"/>
     </row>
     <row r="3" spans="2:15" ht="11.25" customHeight="1">
       <c r="K3" s="102"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
+      <c r="C4" s="203"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="189" t="s">
+      <c r="H4" s="204" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="189"/>
-      <c r="J4" s="189"/>
+      <c r="I4" s="204"/>
+      <c r="J4" s="204"/>
       <c r="K4" s="145"/>
-      <c r="L4" s="192" t="s">
+      <c r="L4" s="184" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="192"/>
+      <c r="M4" s="184"/>
     </row>
     <row r="5" spans="2:15">
       <c r="C5" s="2" t="s">
@@ -4625,10 +4797,10 @@
       </c>
     </row>
     <row r="10" spans="2:15">
-      <c r="C10" s="196" t="s">
+      <c r="C10" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="197"/>
+      <c r="D10" s="190"/>
       <c r="E10" s="64">
         <v>14</v>
       </c>
@@ -4661,7 +4833,7 @@
       </c>
       <c r="F12" s="6" t="str">
         <f>IFERROR(VLOOKUP($G$2,Classe!$A$3:$G$22,5),"")</f>
-        <v>-</v>
+        <v/>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="144"/>
@@ -4671,10 +4843,10 @@
       <c r="L12" s="12"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="C13" s="196" t="s">
+      <c r="C13" s="189" t="s">
         <v>280</v>
       </c>
-      <c r="D13" s="197"/>
+      <c r="D13" s="190"/>
       <c r="E13" s="40"/>
       <c r="F13" s="10"/>
       <c r="G13" s="12"/>
@@ -4718,17 +4890,17 @@
         <v>25</v>
       </c>
       <c r="I16" s="14"/>
-      <c r="L16" s="218" t="s">
+      <c r="L16" s="181" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="218"/>
-      <c r="N16" s="218"/>
+      <c r="M16" s="181"/>
+      <c r="N16" s="181"/>
     </row>
     <row r="17" spans="3:14">
-      <c r="C17" s="190">
+      <c r="C17" s="205">
         <v>11</v>
       </c>
-      <c r="D17" s="191"/>
+      <c r="D17" s="206"/>
       <c r="E17" s="109"/>
       <c r="F17" s="110"/>
       <c r="G17" s="110"/>
@@ -4737,10 +4909,10 @@
       <c r="L17" s="38">
         <v>1</v>
       </c>
-      <c r="M17" s="219" t="s">
+      <c r="M17" s="182" t="s">
         <v>55</v>
       </c>
-      <c r="N17" s="168"/>
+      <c r="N17" s="183"/>
     </row>
     <row r="18" spans="3:14">
       <c r="C18" s="103" t="s">
@@ -4763,25 +4935,25 @@
       <c r="L18" s="39">
         <v>0</v>
       </c>
-      <c r="M18" s="168" t="s">
+      <c r="M18" s="183" t="s">
         <v>56</v>
       </c>
-      <c r="N18" s="168"/>
+      <c r="N18" s="183"/>
     </row>
     <row r="19" spans="3:14">
-      <c r="C19" s="194">
+      <c r="C19" s="187">
         <v>10</v>
       </c>
-      <c r="D19" s="195"/>
+      <c r="D19" s="188"/>
       <c r="E19" s="106">
         <v>10</v>
       </c>
       <c r="F19" s="107">
         <v>8</v>
       </c>
-      <c r="G19" s="108">
+      <c r="G19" s="108" t="e">
         <f>G2</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H19" s="113"/>
       <c r="I19" s="12"/>
@@ -4790,52 +4962,52 @@
       <c r="L19" s="39">
         <v>0</v>
       </c>
-      <c r="M19" s="168" t="s">
+      <c r="M19" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="N19" s="168"/>
+      <c r="N19" s="183"/>
     </row>
     <row r="20" spans="3:14">
       <c r="C20" s="114" t="s">
         <v>327</v>
       </c>
       <c r="D20" s="115"/>
-      <c r="E20" s="203" t="s">
+      <c r="E20" s="198" t="s">
         <v>328</v>
       </c>
-      <c r="F20" s="203"/>
+      <c r="F20" s="198"/>
       <c r="G20" s="141" t="s">
         <v>365</v>
       </c>
       <c r="L20" s="39">
         <v>0</v>
       </c>
-      <c r="M20" s="168" t="s">
+      <c r="M20" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="168"/>
+      <c r="N20" s="183"/>
     </row>
     <row r="21" spans="3:14">
-      <c r="C21" s="194">
-        <v>0</v>
-      </c>
-      <c r="D21" s="195"/>
-      <c r="E21" s="200" t="str">
+      <c r="C21" s="187">
+        <v>0</v>
+      </c>
+      <c r="D21" s="188"/>
+      <c r="E21" s="195" t="e">
         <f>VLOOKUP($G$2,Classe!$A$3:$F$22,4)</f>
-        <v>-</v>
-      </c>
-      <c r="F21" s="200"/>
-      <c r="G21" s="142" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="F21" s="195"/>
+      <c r="G21" s="142" t="e">
         <f>VLOOKUP($G$2,Classe!A3:G22,7)</f>
-        <v>-</v>
+        <v>#VALUE!</v>
       </c>
       <c r="L21" s="40">
         <v>0</v>
       </c>
-      <c r="M21" s="220" t="s">
+      <c r="M21" s="185" t="s">
         <v>59</v>
       </c>
-      <c r="N21" s="221"/>
+      <c r="N21" s="186"/>
     </row>
     <row r="22" spans="3:14">
       <c r="C22" s="116"/>
@@ -4847,20 +5019,20 @@
         <v>285</v>
       </c>
       <c r="D24" s="89"/>
-      <c r="E24" s="208" t="s">
+      <c r="E24" s="164" t="s">
         <v>261</v>
       </c>
-      <c r="F24" s="208"/>
-      <c r="G24" s="208"/>
+      <c r="F24" s="164"/>
+      <c r="G24" s="164"/>
       <c r="J24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K24" s="209" t="s">
+      <c r="K24" s="165" t="s">
         <v>64</v>
       </c>
-      <c r="L24" s="210"/>
-      <c r="M24" s="210"/>
-      <c r="N24" s="211"/>
+      <c r="L24" s="166"/>
+      <c r="M24" s="166"/>
+      <c r="N24" s="167"/>
     </row>
     <row r="25" spans="3:14">
       <c r="C25" s="155" t="s">
@@ -4869,16 +5041,16 @@
       <c r="D25" s="156" t="s">
         <v>362</v>
       </c>
-      <c r="E25" s="201"/>
-      <c r="F25" s="201"/>
-      <c r="G25" s="202"/>
+      <c r="E25" s="196"/>
+      <c r="F25" s="196"/>
+      <c r="G25" s="197"/>
       <c r="J25" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="K25" s="181"/>
-      <c r="L25" s="182"/>
-      <c r="M25" s="182"/>
-      <c r="N25" s="183"/>
+      <c r="K25" s="168"/>
+      <c r="L25" s="169"/>
+      <c r="M25" s="169"/>
+      <c r="N25" s="170"/>
     </row>
     <row r="26" spans="3:14" ht="14.25" customHeight="1">
       <c r="C26" s="157" t="s">
@@ -4887,24 +5059,24 @@
       <c r="D26" s="158" t="s">
         <v>361</v>
       </c>
-      <c r="E26" s="184" t="str">
+      <c r="E26" s="179" t="e">
         <f>VLOOKUP($G$2,Classe!A3:F22,3,FALSE)</f>
-        <v>1d4</v>
-      </c>
-      <c r="F26" s="184"/>
-      <c r="G26" s="185"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F26" s="179"/>
+      <c r="G26" s="180"/>
       <c r="J26" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="K26" s="179" t="str">
+      <c r="K26" s="171" t="str">
         <f>VLOOKUP($K24,[1]Armes!$A$2:$F$42,3)</f>
         <v>1d6 contondant</v>
       </c>
-      <c r="L26" s="180"/>
-      <c r="M26" s="180"/>
-      <c r="N26" s="120">
+      <c r="L26" s="172"/>
+      <c r="M26" s="172"/>
+      <c r="N26" s="120" t="e">
         <f>IF(IFERROR(INDEX(Maitrise!$A$2:$B$40,MATCH($K$24,Maitrise!$B$2:$B$40,0),1),0)=1,Maitrise!$P$2,"")</f>
-        <v>2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="3:14" ht="15" customHeight="1">
@@ -4914,21 +5086,21 @@
       <c r="D27" s="158" t="s">
         <v>281</v>
       </c>
-      <c r="E27" s="184" t="s">
+      <c r="E27" s="179" t="s">
         <v>283</v>
       </c>
-      <c r="F27" s="184"/>
-      <c r="G27" s="185"/>
-      <c r="J27" s="169" t="s">
+      <c r="F27" s="179"/>
+      <c r="G27" s="180"/>
+      <c r="J27" s="208" t="s">
         <v>158</v>
       </c>
-      <c r="K27" s="212" t="str">
+      <c r="K27" s="173" t="str">
         <f>VLOOKUP($K24,[1]Armes!$A$2:$F$42,4,FALSE)&amp;" - "&amp;VLOOKUP($K24,[1]Armes!$A$2:$F$42,6,FALSE)</f>
         <v>1d6  - 2 kg</v>
       </c>
-      <c r="L27" s="213"/>
-      <c r="M27" s="213"/>
-      <c r="N27" s="214"/>
+      <c r="L27" s="174"/>
+      <c r="M27" s="174"/>
+      <c r="N27" s="175"/>
     </row>
     <row r="28" spans="3:14">
       <c r="C28" s="159">
@@ -4937,137 +5109,137 @@
       <c r="D28" s="158" t="s">
         <v>282</v>
       </c>
-      <c r="E28" s="184" t="s">
+      <c r="E28" s="179" t="s">
         <v>326</v>
       </c>
-      <c r="F28" s="184"/>
-      <c r="G28" s="185"/>
-      <c r="J28" s="170"/>
-      <c r="K28" s="212"/>
-      <c r="L28" s="213"/>
-      <c r="M28" s="213"/>
-      <c r="N28" s="214"/>
+      <c r="F28" s="179"/>
+      <c r="G28" s="180"/>
+      <c r="J28" s="209"/>
+      <c r="K28" s="173"/>
+      <c r="L28" s="174"/>
+      <c r="M28" s="174"/>
+      <c r="N28" s="175"/>
     </row>
     <row r="29" spans="3:14">
       <c r="C29" s="39"/>
       <c r="D29" s="85"/>
-      <c r="E29" s="184"/>
-      <c r="F29" s="184"/>
-      <c r="G29" s="185"/>
-      <c r="J29" s="171"/>
-      <c r="K29" s="215"/>
-      <c r="L29" s="216"/>
-      <c r="M29" s="216"/>
-      <c r="N29" s="217"/>
+      <c r="E29" s="179"/>
+      <c r="F29" s="179"/>
+      <c r="G29" s="180"/>
+      <c r="J29" s="210"/>
+      <c r="K29" s="176"/>
+      <c r="L29" s="177"/>
+      <c r="M29" s="177"/>
+      <c r="N29" s="178"/>
     </row>
     <row r="30" spans="3:14">
       <c r="C30" s="39"/>
       <c r="D30" s="85"/>
-      <c r="E30" s="184"/>
-      <c r="F30" s="184"/>
-      <c r="G30" s="185"/>
+      <c r="E30" s="179"/>
+      <c r="F30" s="179"/>
+      <c r="G30" s="180"/>
     </row>
     <row r="31" spans="3:14">
       <c r="C31" s="39"/>
       <c r="D31" s="85"/>
-      <c r="E31" s="184"/>
-      <c r="F31" s="184"/>
-      <c r="G31" s="185"/>
+      <c r="E31" s="179"/>
+      <c r="F31" s="179"/>
+      <c r="G31" s="180"/>
       <c r="J31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K31" s="209" t="s">
+      <c r="K31" s="165" t="s">
         <v>330</v>
       </c>
-      <c r="L31" s="210"/>
-      <c r="M31" s="210"/>
-      <c r="N31" s="211"/>
+      <c r="L31" s="166"/>
+      <c r="M31" s="166"/>
+      <c r="N31" s="167"/>
     </row>
     <row r="32" spans="3:14">
       <c r="C32" s="39"/>
       <c r="D32" s="85"/>
-      <c r="E32" s="184"/>
-      <c r="F32" s="184"/>
-      <c r="G32" s="185"/>
+      <c r="E32" s="179"/>
+      <c r="F32" s="179"/>
+      <c r="G32" s="180"/>
       <c r="J32" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="K32" s="181"/>
-      <c r="L32" s="182"/>
-      <c r="M32" s="182"/>
-      <c r="N32" s="183"/>
+      <c r="K32" s="168"/>
+      <c r="L32" s="169"/>
+      <c r="M32" s="169"/>
+      <c r="N32" s="170"/>
     </row>
     <row r="33" spans="3:14" ht="15" customHeight="1">
       <c r="C33" s="39"/>
       <c r="D33" s="85"/>
-      <c r="E33" s="184"/>
-      <c r="F33" s="184"/>
-      <c r="G33" s="185"/>
+      <c r="E33" s="179"/>
+      <c r="F33" s="179"/>
+      <c r="G33" s="180"/>
       <c r="J33" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="K33" s="179" t="str">
+      <c r="K33" s="171" t="str">
         <f>VLOOKUP($K31,[1]Armes!$A$2:$F$42,3)</f>
         <v>1d4 tranchant</v>
       </c>
-      <c r="L33" s="180"/>
-      <c r="M33" s="180"/>
-      <c r="N33" s="120">
+      <c r="L33" s="172"/>
+      <c r="M33" s="172"/>
+      <c r="N33" s="120" t="e">
         <f>IF(IFERROR(INDEX(Maitrise!$A$2:$B$40,MATCH($K$31,Maitrise!$B$2:$B$40,0),1),0)=1,Maitrise!$P$2,"")</f>
-        <v>2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="3:14" ht="16.5" customHeight="1">
       <c r="C34" s="39"/>
       <c r="D34" s="85"/>
-      <c r="E34" s="184"/>
-      <c r="F34" s="184"/>
-      <c r="G34" s="185"/>
+      <c r="E34" s="179"/>
+      <c r="F34" s="179"/>
+      <c r="G34" s="180"/>
       <c r="J34" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="K34" s="178">
+      <c r="K34" s="217">
         <v>10</v>
       </c>
-      <c r="L34" s="163"/>
-      <c r="M34" s="163"/>
-      <c r="N34" s="164"/>
+      <c r="L34" s="193"/>
+      <c r="M34" s="193"/>
+      <c r="N34" s="194"/>
     </row>
     <row r="35" spans="3:14" ht="15" customHeight="1">
       <c r="C35" s="39"/>
       <c r="D35" s="85"/>
-      <c r="E35" s="184"/>
-      <c r="F35" s="184"/>
-      <c r="G35" s="185"/>
-      <c r="J35" s="169" t="s">
+      <c r="E35" s="179"/>
+      <c r="F35" s="179"/>
+      <c r="G35" s="180"/>
+      <c r="J35" s="208" t="s">
         <v>158</v>
       </c>
-      <c r="K35" s="172" t="str">
+      <c r="K35" s="211" t="str">
         <f>VLOOKUP($K31,[1]Armes!$A$2:$F$42,4,FALSE)&amp;" - "&amp;VLOOKUP($K31,[1]Armes!$A$2:$F$42,6,FALSE)</f>
         <v>1d4  - 0 g</v>
       </c>
-      <c r="L35" s="173"/>
-      <c r="M35" s="173"/>
-      <c r="N35" s="174"/>
+      <c r="L35" s="212"/>
+      <c r="M35" s="212"/>
+      <c r="N35" s="213"/>
     </row>
     <row r="36" spans="3:14">
       <c r="C36" s="40"/>
       <c r="D36" s="83"/>
-      <c r="E36" s="204"/>
-      <c r="F36" s="204"/>
-      <c r="G36" s="205"/>
-      <c r="J36" s="170"/>
-      <c r="K36" s="172"/>
-      <c r="L36" s="173"/>
-      <c r="M36" s="173"/>
-      <c r="N36" s="174"/>
+      <c r="E36" s="199"/>
+      <c r="F36" s="199"/>
+      <c r="G36" s="200"/>
+      <c r="J36" s="209"/>
+      <c r="K36" s="211"/>
+      <c r="L36" s="212"/>
+      <c r="M36" s="212"/>
+      <c r="N36" s="213"/>
     </row>
     <row r="37" spans="3:14">
-      <c r="J37" s="171"/>
-      <c r="K37" s="175"/>
-      <c r="L37" s="176"/>
-      <c r="M37" s="176"/>
-      <c r="N37" s="177"/>
+      <c r="J37" s="210"/>
+      <c r="K37" s="214"/>
+      <c r="L37" s="215"/>
+      <c r="M37" s="215"/>
+      <c r="N37" s="216"/>
     </row>
     <row r="38" spans="3:14">
       <c r="C38" s="95" t="s">
@@ -5086,121 +5258,121 @@
       <c r="D39" s="96">
         <v>0</v>
       </c>
-      <c r="E39" s="198"/>
-      <c r="F39" s="198"/>
-      <c r="G39" s="199"/>
+      <c r="E39" s="191"/>
+      <c r="F39" s="191"/>
+      <c r="G39" s="192"/>
       <c r="J39" s="154"/>
-      <c r="K39" s="165"/>
-      <c r="L39" s="165"/>
-      <c r="M39" s="165"/>
-      <c r="N39" s="165"/>
+      <c r="K39" s="220"/>
+      <c r="L39" s="220"/>
+      <c r="M39" s="220"/>
+      <c r="N39" s="220"/>
     </row>
     <row r="40" spans="3:14">
       <c r="C40" s="99"/>
       <c r="D40" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="E40" s="163"/>
-      <c r="F40" s="163"/>
-      <c r="G40" s="164"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="193"/>
+      <c r="G40" s="194"/>
       <c r="J40" s="154"/>
-      <c r="K40" s="167"/>
-      <c r="L40" s="167"/>
-      <c r="M40" s="167"/>
-      <c r="N40" s="167"/>
+      <c r="K40" s="222"/>
+      <c r="L40" s="222"/>
+      <c r="M40" s="222"/>
+      <c r="N40" s="222"/>
     </row>
     <row r="41" spans="3:14">
       <c r="C41" s="99"/>
       <c r="D41" s="97" t="s">
         <v>161</v>
       </c>
-      <c r="E41" s="163"/>
-      <c r="F41" s="163"/>
-      <c r="G41" s="164"/>
+      <c r="E41" s="193"/>
+      <c r="F41" s="193"/>
+      <c r="G41" s="194"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="154"/>
-      <c r="K41" s="166"/>
-      <c r="L41" s="166"/>
-      <c r="M41" s="166"/>
-      <c r="N41" s="166"/>
+      <c r="K41" s="221"/>
+      <c r="L41" s="221"/>
+      <c r="M41" s="221"/>
+      <c r="N41" s="221"/>
     </row>
     <row r="42" spans="3:14">
       <c r="C42" s="99"/>
       <c r="D42" s="97" t="s">
         <v>166</v>
       </c>
-      <c r="E42" s="163"/>
-      <c r="F42" s="163"/>
-      <c r="G42" s="164"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="193"/>
+      <c r="G42" s="194"/>
     </row>
     <row r="43" spans="3:14">
       <c r="C43" s="99"/>
       <c r="D43" s="97" t="s">
         <v>163</v>
       </c>
-      <c r="E43" s="163"/>
-      <c r="F43" s="163"/>
-      <c r="G43" s="164"/>
+      <c r="E43" s="193"/>
+      <c r="F43" s="193"/>
+      <c r="G43" s="194"/>
     </row>
     <row r="44" spans="3:14">
       <c r="C44" s="99"/>
       <c r="D44" s="97" t="s">
         <v>167</v>
       </c>
-      <c r="E44" s="163"/>
-      <c r="F44" s="163"/>
-      <c r="G44" s="164"/>
+      <c r="E44" s="193"/>
+      <c r="F44" s="193"/>
+      <c r="G44" s="194"/>
     </row>
     <row r="45" spans="3:14">
       <c r="C45" s="99"/>
       <c r="D45" s="97" t="s">
         <v>164</v>
       </c>
-      <c r="E45" s="163"/>
-      <c r="F45" s="163"/>
-      <c r="G45" s="164"/>
+      <c r="E45" s="193"/>
+      <c r="F45" s="193"/>
+      <c r="G45" s="194"/>
     </row>
     <row r="46" spans="3:14">
       <c r="C46" s="100"/>
       <c r="D46" s="97" t="s">
         <v>168</v>
       </c>
-      <c r="E46" s="163"/>
-      <c r="F46" s="163"/>
-      <c r="G46" s="164"/>
+      <c r="E46" s="193"/>
+      <c r="F46" s="193"/>
+      <c r="G46" s="194"/>
     </row>
     <row r="47" spans="3:14">
       <c r="C47" s="99"/>
       <c r="D47" s="97" t="s">
         <v>165</v>
       </c>
-      <c r="E47" s="163"/>
-      <c r="F47" s="163"/>
-      <c r="G47" s="164"/>
+      <c r="E47" s="193"/>
+      <c r="F47" s="193"/>
+      <c r="G47" s="194"/>
     </row>
     <row r="48" spans="3:14">
       <c r="C48" s="99"/>
       <c r="D48" s="97" t="s">
         <v>169</v>
       </c>
-      <c r="E48" s="163"/>
-      <c r="F48" s="163"/>
-      <c r="G48" s="164"/>
+      <c r="E48" s="193"/>
+      <c r="F48" s="193"/>
+      <c r="G48" s="194"/>
     </row>
     <row r="49" spans="3:15">
       <c r="C49" s="99"/>
       <c r="D49" s="147"/>
-      <c r="E49" s="163"/>
-      <c r="F49" s="163"/>
-      <c r="G49" s="164"/>
+      <c r="E49" s="193"/>
+      <c r="F49" s="193"/>
+      <c r="G49" s="194"/>
     </row>
     <row r="50" spans="3:15">
       <c r="C50" s="101"/>
       <c r="D50" s="160"/>
-      <c r="E50" s="161"/>
-      <c r="F50" s="161"/>
-      <c r="G50" s="162"/>
+      <c r="E50" s="218"/>
+      <c r="F50" s="218"/>
+      <c r="G50" s="219"/>
     </row>
     <row r="56" spans="3:15">
       <c r="I56" s="146"/>
@@ -5287,6 +5459,50 @@
   </sheetData>
   <sheetProtection sheet="1" scenarios="1"/>
   <mergeCells count="60">
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="J27:J29"/>
+    <mergeCell ref="K35:N37"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="K24:N24"/>
@@ -5303,53 +5519,9 @@
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:G28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="J27:J29"/>
-    <mergeCell ref="K35:N37"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="J35:J37"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="K39:N39"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:I10">
-    <cfRule type="expression" dxfId="5" priority="27">
+    <cfRule type="expression" dxfId="9" priority="27">
       <formula>$J5=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5382,12 +5554,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5:M10 M17:M21">
-    <cfRule type="expression" dxfId="4" priority="39">
+    <cfRule type="expression" dxfId="8" priority="39">
       <formula>$L5=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:I2">
-    <cfRule type="expression" dxfId="3" priority="40">
+    <cfRule type="expression" dxfId="7" priority="40">
       <formula>$H$2&gt;=$I$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5406,34 +5578,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:E36">
-    <cfRule type="expression" dxfId="2" priority="45">
+    <cfRule type="expression" dxfId="6" priority="45">
       <formula>$C25=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:F10 E12:E13 L59 K34 E17:I17 G19:I19 E19 C39:C50 C28 E39:E50">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:F10 E12:E13 L59 K34 E17:I17 G19:I19 E19 C39:C50 C28 E39:E50" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>50</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17:D17">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17:D17" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L17:L21 L5:L10">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L17:L21 L5:L10" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:D19 C21">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:D19 C21" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
       <formula2>E19</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>0</formula1>
       <formula2>#REF!</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C1:D1" r:id="rId1" display="Race"/>
+    <hyperlink ref="C1:D1" r:id="rId1" display="Race" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -5509,31 +5681,31 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>Listes!$C$2:$C$11</xm:f>
           </x14:formula1>
           <xm:sqref>F19</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>Listes!$A$2:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>C2:D2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>Classe!$I$2:$I$13</xm:f>
           </x14:formula1>
           <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>Maitrise!$B$1:$B$29</xm:f>
           </x14:formula1>
           <xm:sqref>I56 K24</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
           <x14:formula1>
             <xm:f>Maitrise!$B$30:$B$40</xm:f>
           </x14:formula1>
@@ -5546,7 +5718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" workbookViewId="0">
@@ -5664,7 +5836,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="222" t="s">
+      <c r="A18" s="223" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="47" t="s">
@@ -5672,13 +5844,13 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="222"/>
+      <c r="A19" s="223"/>
       <c r="B19" s="48" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="222"/>
+      <c r="A20" s="223"/>
       <c r="B20" s="52" t="s">
         <v>284</v>
       </c>
@@ -5693,7 +5865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5729,22 +5901,22 @@
       <c r="B1" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="223" t="s">
+      <c r="D1" s="224" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="224"/>
-      <c r="G1" s="223" t="s">
+      <c r="E1" s="225"/>
+      <c r="G1" s="224" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="224"/>
-      <c r="I1" s="223" t="s">
+      <c r="H1" s="225"/>
+      <c r="I1" s="224" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="224"/>
-      <c r="K1" s="223" t="s">
+      <c r="J1" s="225"/>
+      <c r="K1" s="224" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="224"/>
+      <c r="L1" s="225"/>
       <c r="M1" s="32"/>
       <c r="N1" s="33" t="s">
         <v>133</v>
@@ -5792,9 +5964,9 @@
         <v>134</v>
       </c>
       <c r="O2" s="12"/>
-      <c r="P2" s="90">
+      <c r="P2" s="90" t="e">
         <f>VLOOKUP(Principal!$G$2,[1]Niveaux!$A$2:$C$21,3)</f>
-        <v>2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -5882,10 +6054,10 @@
       <c r="B5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="225" t="s">
+      <c r="D5" s="226" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="224"/>
+      <c r="E5" s="225"/>
       <c r="G5" s="39">
         <v>0</v>
       </c>
@@ -6070,10 +6242,10 @@
       <c r="B11" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="225" t="s">
+      <c r="D11" s="226" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="224"/>
+      <c r="E11" s="225"/>
       <c r="G11" s="39">
         <v>0</v>
       </c>
@@ -6205,10 +6377,10 @@
       <c r="B16" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="225" t="s">
+      <c r="D16" s="226" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="224"/>
+      <c r="E16" s="225"/>
       <c r="G16" s="39"/>
       <c r="H16" s="8"/>
       <c r="I16" s="39"/>
@@ -6581,12 +6753,12 @@
     <mergeCell ref="D5:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="N2:N19 E6:E10 B13:B29 B2:B11 B31:B34 B36:B40 E2:E4 E12:E15 E17:E19 L2:L19 J2:J19 H2:H19">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>A2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:A29 D6:D10 M2:M19 A2:A11 K2:K19 A31:A34 A36:A40 D2:D4 L23:L24 D12:D15 D17:D19 G2:G19 L36:L43 I2:I19 N29:N43">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:A29 D6:D10 M2:M19 A2:A11 K2:K19 A31:A34 A36:A40 D2:D4 L23:L24 D12:D15 D17:D19 G2:G19 L36:L43 I2:I19 N29:N43" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -6678,7 +6850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" workbookViewId="0">
@@ -6694,10 +6866,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="224" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="224"/>
+      <c r="B1" s="225"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:9">
@@ -8637,7 +8809,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:C81">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A2=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8672,7 +8844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
@@ -8743,10 +8915,10 @@
       <c r="F2" s="43">
         <v>0</v>
       </c>
-      <c r="H2" s="233"/>
-      <c r="I2" s="234"/>
-      <c r="J2" s="234"/>
-      <c r="K2" s="235"/>
+      <c r="H2" s="229"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="231"/>
       <c r="L2" s="67">
         <v>0</v>
       </c>
@@ -8758,245 +8930,275 @@
       <c r="A3" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="230" t="s">
+      <c r="B3" s="234" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="230"/>
-      <c r="D3" s="230"/>
-      <c r="E3" s="230"/>
-      <c r="F3" s="231"/>
+      <c r="C3" s="234"/>
+      <c r="D3" s="234"/>
+      <c r="E3" s="234"/>
+      <c r="F3" s="235"/>
       <c r="H3" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="I3" s="232" t="s">
+      <c r="I3" s="236" t="s">
         <v>261</v>
       </c>
-      <c r="J3" s="232"/>
+      <c r="J3" s="236"/>
       <c r="K3" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="230" t="s">
+      <c r="L3" s="234" t="s">
         <v>261</v>
       </c>
-      <c r="M3" s="231"/>
+      <c r="M3" s="235"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="39"/>
-      <c r="B4" s="226"/>
-      <c r="C4" s="226"/>
-      <c r="D4" s="226"/>
-      <c r="E4" s="226"/>
-      <c r="F4" s="227"/>
+      <c r="B4" s="232"/>
+      <c r="C4" s="232"/>
+      <c r="D4" s="232"/>
+      <c r="E4" s="232"/>
+      <c r="F4" s="233"/>
       <c r="H4" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="I4" s="226"/>
-      <c r="J4" s="227"/>
+      <c r="I4" s="232"/>
+      <c r="J4" s="233"/>
       <c r="K4" s="39"/>
-      <c r="L4" s="226"/>
-      <c r="M4" s="227"/>
+      <c r="L4" s="232"/>
+      <c r="M4" s="233"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="39"/>
-      <c r="B5" s="226"/>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="226"/>
-      <c r="F5" s="227"/>
+      <c r="B5" s="232"/>
+      <c r="C5" s="232"/>
+      <c r="D5" s="232"/>
+      <c r="E5" s="232"/>
+      <c r="F5" s="233"/>
       <c r="H5" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="I5" s="226"/>
-      <c r="J5" s="227"/>
+      <c r="I5" s="232"/>
+      <c r="J5" s="233"/>
       <c r="K5" s="39"/>
-      <c r="L5" s="226"/>
-      <c r="M5" s="227"/>
+      <c r="L5" s="232"/>
+      <c r="M5" s="233"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="39"/>
-      <c r="B6" s="226"/>
-      <c r="C6" s="226"/>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="227"/>
+      <c r="B6" s="232"/>
+      <c r="C6" s="232"/>
+      <c r="D6" s="232"/>
+      <c r="E6" s="232"/>
+      <c r="F6" s="233"/>
       <c r="H6" s="39"/>
-      <c r="I6" s="226"/>
-      <c r="J6" s="227"/>
+      <c r="I6" s="232"/>
+      <c r="J6" s="233"/>
       <c r="K6" s="39"/>
-      <c r="L6" s="226"/>
-      <c r="M6" s="227"/>
+      <c r="L6" s="232"/>
+      <c r="M6" s="233"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="39"/>
-      <c r="B7" s="226"/>
-      <c r="C7" s="226"/>
-      <c r="D7" s="226"/>
-      <c r="E7" s="226"/>
-      <c r="F7" s="227"/>
+      <c r="B7" s="232"/>
+      <c r="C7" s="232"/>
+      <c r="D7" s="232"/>
+      <c r="E7" s="232"/>
+      <c r="F7" s="233"/>
       <c r="H7" s="39"/>
-      <c r="I7" s="226"/>
-      <c r="J7" s="227"/>
+      <c r="I7" s="232"/>
+      <c r="J7" s="233"/>
       <c r="K7" s="39"/>
-      <c r="L7" s="226"/>
-      <c r="M7" s="227"/>
+      <c r="L7" s="232"/>
+      <c r="M7" s="233"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="39"/>
-      <c r="B8" s="226"/>
-      <c r="C8" s="226"/>
-      <c r="D8" s="226"/>
-      <c r="E8" s="226"/>
-      <c r="F8" s="227"/>
+      <c r="B8" s="232"/>
+      <c r="C8" s="232"/>
+      <c r="D8" s="232"/>
+      <c r="E8" s="232"/>
+      <c r="F8" s="233"/>
       <c r="H8" s="39"/>
-      <c r="I8" s="226"/>
-      <c r="J8" s="227"/>
+      <c r="I8" s="232"/>
+      <c r="J8" s="233"/>
       <c r="K8" s="75" t="s">
         <v>267</v>
       </c>
-      <c r="L8" s="230" t="s">
+      <c r="L8" s="234" t="s">
         <v>261</v>
       </c>
-      <c r="M8" s="231"/>
+      <c r="M8" s="235"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="39"/>
-      <c r="B9" s="226"/>
-      <c r="C9" s="226"/>
-      <c r="D9" s="226"/>
-      <c r="E9" s="226"/>
-      <c r="F9" s="227"/>
+      <c r="B9" s="232"/>
+      <c r="C9" s="232"/>
+      <c r="D9" s="232"/>
+      <c r="E9" s="232"/>
+      <c r="F9" s="233"/>
       <c r="H9" s="39"/>
-      <c r="I9" s="226"/>
-      <c r="J9" s="227"/>
+      <c r="I9" s="232"/>
+      <c r="J9" s="233"/>
       <c r="K9" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="L9" s="226"/>
-      <c r="M9" s="227"/>
+      <c r="L9" s="232"/>
+      <c r="M9" s="233"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="39"/>
-      <c r="B10" s="226"/>
-      <c r="C10" s="226"/>
-      <c r="D10" s="226"/>
-      <c r="E10" s="226"/>
-      <c r="F10" s="227"/>
+      <c r="B10" s="232"/>
+      <c r="C10" s="232"/>
+      <c r="D10" s="232"/>
+      <c r="E10" s="232"/>
+      <c r="F10" s="233"/>
       <c r="H10" s="39"/>
-      <c r="I10" s="226"/>
-      <c r="J10" s="227"/>
+      <c r="I10" s="232"/>
+      <c r="J10" s="233"/>
       <c r="K10" s="39"/>
-      <c r="L10" s="226"/>
-      <c r="M10" s="227"/>
+      <c r="L10" s="232"/>
+      <c r="M10" s="233"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="39"/>
-      <c r="B11" s="226"/>
-      <c r="C11" s="226"/>
-      <c r="D11" s="226"/>
-      <c r="E11" s="226"/>
-      <c r="F11" s="227"/>
+      <c r="B11" s="232"/>
+      <c r="C11" s="232"/>
+      <c r="D11" s="232"/>
+      <c r="E11" s="232"/>
+      <c r="F11" s="233"/>
       <c r="H11" s="39"/>
-      <c r="I11" s="226"/>
-      <c r="J11" s="227"/>
+      <c r="I11" s="232"/>
+      <c r="J11" s="233"/>
       <c r="K11" s="39"/>
-      <c r="L11" s="226"/>
-      <c r="M11" s="227"/>
+      <c r="L11" s="232"/>
+      <c r="M11" s="233"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="39"/>
-      <c r="B12" s="226"/>
-      <c r="C12" s="226"/>
-      <c r="D12" s="226"/>
-      <c r="E12" s="226"/>
-      <c r="F12" s="227"/>
+      <c r="B12" s="232"/>
+      <c r="C12" s="232"/>
+      <c r="D12" s="232"/>
+      <c r="E12" s="232"/>
+      <c r="F12" s="233"/>
       <c r="H12" s="39"/>
-      <c r="I12" s="226"/>
-      <c r="J12" s="227"/>
+      <c r="I12" s="232"/>
+      <c r="J12" s="233"/>
       <c r="K12" s="39"/>
-      <c r="L12" s="226"/>
-      <c r="M12" s="227"/>
+      <c r="L12" s="232"/>
+      <c r="M12" s="233"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="39"/>
-      <c r="B13" s="226"/>
-      <c r="C13" s="226"/>
-      <c r="D13" s="226"/>
-      <c r="E13" s="226"/>
-      <c r="F13" s="227"/>
+      <c r="B13" s="232"/>
+      <c r="C13" s="232"/>
+      <c r="D13" s="232"/>
+      <c r="E13" s="232"/>
+      <c r="F13" s="233"/>
       <c r="H13" s="39"/>
-      <c r="I13" s="226"/>
-      <c r="J13" s="227"/>
+      <c r="I13" s="232"/>
+      <c r="J13" s="233"/>
       <c r="K13" s="75" t="s">
         <v>268</v>
       </c>
-      <c r="L13" s="230" t="s">
+      <c r="L13" s="234" t="s">
         <v>261</v>
       </c>
-      <c r="M13" s="231"/>
+      <c r="M13" s="235"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="39"/>
-      <c r="B14" s="226"/>
-      <c r="C14" s="226"/>
-      <c r="D14" s="226"/>
-      <c r="E14" s="226"/>
-      <c r="F14" s="227"/>
+      <c r="B14" s="232"/>
+      <c r="C14" s="232"/>
+      <c r="D14" s="232"/>
+      <c r="E14" s="232"/>
+      <c r="F14" s="233"/>
       <c r="H14" s="39"/>
-      <c r="I14" s="226"/>
-      <c r="J14" s="227"/>
+      <c r="I14" s="232"/>
+      <c r="J14" s="233"/>
       <c r="K14" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="L14" s="226"/>
-      <c r="M14" s="227"/>
+      <c r="L14" s="232"/>
+      <c r="M14" s="233"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="39"/>
-      <c r="B15" s="226"/>
-      <c r="C15" s="226"/>
-      <c r="D15" s="226"/>
-      <c r="E15" s="226"/>
-      <c r="F15" s="227"/>
+      <c r="B15" s="232"/>
+      <c r="C15" s="232"/>
+      <c r="D15" s="232"/>
+      <c r="E15" s="232"/>
+      <c r="F15" s="233"/>
       <c r="H15" s="39"/>
-      <c r="I15" s="226"/>
-      <c r="J15" s="227"/>
+      <c r="I15" s="232"/>
+      <c r="J15" s="233"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="226"/>
-      <c r="M15" s="227"/>
+      <c r="L15" s="232"/>
+      <c r="M15" s="233"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="39"/>
-      <c r="B16" s="226"/>
-      <c r="C16" s="226"/>
-      <c r="D16" s="226"/>
-      <c r="E16" s="226"/>
-      <c r="F16" s="227"/>
+      <c r="B16" s="232"/>
+      <c r="C16" s="232"/>
+      <c r="D16" s="232"/>
+      <c r="E16" s="232"/>
+      <c r="F16" s="233"/>
       <c r="H16" s="39"/>
-      <c r="I16" s="226"/>
-      <c r="J16" s="227"/>
+      <c r="I16" s="232"/>
+      <c r="J16" s="233"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="226"/>
-      <c r="M16" s="227"/>
+      <c r="L16" s="232"/>
+      <c r="M16" s="233"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="40"/>
-      <c r="B17" s="228"/>
-      <c r="C17" s="228"/>
-      <c r="D17" s="228"/>
-      <c r="E17" s="228"/>
-      <c r="F17" s="229"/>
+      <c r="B17" s="227"/>
+      <c r="C17" s="227"/>
+      <c r="D17" s="227"/>
+      <c r="E17" s="227"/>
+      <c r="F17" s="228"/>
       <c r="H17" s="40" t="s">
         <v>265</v>
       </c>
-      <c r="I17" s="228"/>
-      <c r="J17" s="229"/>
+      <c r="I17" s="227"/>
+      <c r="J17" s="228"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="228"/>
-      <c r="M17" s="229"/>
+      <c r="L17" s="227"/>
+      <c r="M17" s="228"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="46">
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="L11:M11"/>
@@ -9013,47 +9215,17 @@
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B16:F16"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 L2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 L2" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>0</formula1>
       <formula2>C2</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 C2 E2:F2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2 C2 E2:F2" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -9064,7 +9236,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" workbookViewId="0">
@@ -9618,7 +9790,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -9628,7 +9800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9746,7 +9918,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
-      <c r="D16" s="236"/>
+      <c r="D16" s="161"/>
     </row>
     <row r="17" ht="18.75" customHeight="1"/>
     <row r="18" ht="15" customHeight="1"/>

</xml_diff>

<commit_message>
Global Layout + Init Damages component
</commit_message>
<xml_diff>
--- a/Personnage.xlsx
+++ b/Personnage.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F84BB75-63C6-4FE2-BBB7-2ED92E2A8034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08723F3-BED9-4C0B-8D17-B75B72325621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -3172,6 +3172,8 @@
       <sheetName val="Classes"/>
       <sheetName val="Capacities"/>
       <sheetName val="Specialisation-capacities"/>
+      <sheetName val="Compétences"/>
+      <sheetName val="Compétences de race"/>
       <sheetName val="Historiques"/>
       <sheetName val="Armes"/>
       <sheetName val="Armures"/>
@@ -3419,16 +3421,13 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
-      <sheetData sheetId="7">
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
         <row r="2">
           <cell r="A2" t="str">
             <v>Armes courantes de corps à corps</v>
           </cell>
-          <cell r="B2"/>
-          <cell r="C2"/>
-          <cell r="D2"/>
-          <cell r="E2"/>
-          <cell r="F2"/>
         </row>
         <row r="3">
           <cell r="A3" t="str">
@@ -3634,11 +3633,6 @@
           <cell r="A13" t="str">
             <v>Armes courantes à distance</v>
           </cell>
-          <cell r="B13"/>
-          <cell r="C13"/>
-          <cell r="D13"/>
-          <cell r="E13"/>
-          <cell r="F13"/>
         </row>
         <row r="14">
           <cell r="A14" t="str">
@@ -3724,11 +3718,6 @@
           <cell r="A18" t="str">
             <v>Armes de guerre de corps à corps</v>
           </cell>
-          <cell r="B18"/>
-          <cell r="C18"/>
-          <cell r="D18"/>
-          <cell r="E18"/>
-          <cell r="F18"/>
         </row>
         <row r="19">
           <cell r="A19" t="str">
@@ -4094,11 +4083,6 @@
           <cell r="A37" t="str">
             <v>Armes de guerre à distance</v>
           </cell>
-          <cell r="B37"/>
-          <cell r="C37"/>
-          <cell r="D37"/>
-          <cell r="E37"/>
-          <cell r="F37"/>
         </row>
         <row r="38">
           <cell r="A38" t="str">
@@ -4167,9 +4151,6 @@
           <cell r="B41" t="str">
             <v>Net</v>
           </cell>
-          <cell r="C41"/>
-          <cell r="D41"/>
-          <cell r="E41"/>
           <cell r="F41" t="str">
             <v>1,5 kg</v>
           </cell>
@@ -4195,8 +4176,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
@@ -4210,6 +4189,8 @@
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
       <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4568,7 +4549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O73"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
@@ -4633,16 +4614,16 @@
       <c r="F2" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="G2" s="44" t="e">
+      <c r="G2" s="44">
         <f>COUNTIFS([1]Niveaux!$B$2:$B$21,"&lt;="&amp;H2)</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="H2" s="45">
         <v>0</v>
       </c>
-      <c r="I2" s="194" t="e">
+      <c r="I2" s="194">
         <f>VLOOKUP($G$2+1,[1]Niveaux!$A$2:$C$21,2)</f>
-        <v>#VALUE!</v>
+        <v>300</v>
       </c>
       <c r="J2" s="194"/>
       <c r="K2" s="207"/>
@@ -4833,7 +4814,7 @@
       </c>
       <c r="F12" s="6" t="str">
         <f>IFERROR(VLOOKUP($G$2,Classe!$A$3:$G$22,5),"")</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="144"/>
@@ -4951,9 +4932,9 @@
       <c r="F19" s="107">
         <v>8</v>
       </c>
-      <c r="G19" s="108" t="e">
+      <c r="G19" s="108">
         <f>G2</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="H19" s="113"/>
       <c r="I19" s="12"/>
@@ -4992,14 +4973,14 @@
         <v>0</v>
       </c>
       <c r="D21" s="196"/>
-      <c r="E21" s="201" t="e">
+      <c r="E21" s="201" t="str">
         <f>VLOOKUP($G$2,Classe!$A$3:$F$22,4)</f>
-        <v>#VALUE!</v>
+        <v>-</v>
       </c>
       <c r="F21" s="201"/>
-      <c r="G21" s="142" t="e">
+      <c r="G21" s="142" t="str">
         <f>VLOOKUP($G$2,Classe!A3:G22,7)</f>
-        <v>#VALUE!</v>
+        <v>-</v>
       </c>
       <c r="L21" s="40">
         <v>0</v>
@@ -5059,9 +5040,9 @@
       <c r="D26" s="158" t="s">
         <v>361</v>
       </c>
-      <c r="E26" s="185" t="e">
+      <c r="E26" s="185" t="str">
         <f>VLOOKUP($G$2,Classe!A3:F22,3,FALSE)</f>
-        <v>#VALUE!</v>
+        <v>1d4</v>
       </c>
       <c r="F26" s="185"/>
       <c r="G26" s="186"/>
@@ -5074,9 +5055,9 @@
       </c>
       <c r="L26" s="181"/>
       <c r="M26" s="181"/>
-      <c r="N26" s="120" t="e">
+      <c r="N26" s="120">
         <f>IF(IFERROR(INDEX(Maitrise!$A$2:$B$40,MATCH($K$24,Maitrise!$B$2:$B$40,0),1),0)=1,Maitrise!$P$2,"")</f>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="3:14" ht="15" customHeight="1">
@@ -5184,9 +5165,9 @@
       </c>
       <c r="L33" s="181"/>
       <c r="M33" s="181"/>
-      <c r="N33" s="120" t="e">
+      <c r="N33" s="120">
         <f>IF(IFERROR(INDEX(Maitrise!$A$2:$B$40,MATCH($K$31,Maitrise!$B$2:$B$40,0),1),0)=1,Maitrise!$P$2,"")</f>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="3:14" ht="16.5" customHeight="1">
@@ -5721,7 +5702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" workbookViewId="0">
+    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -5964,9 +5945,9 @@
         <v>134</v>
       </c>
       <c r="O2" s="12"/>
-      <c r="P2" s="90" t="e">
+      <c r="P2" s="90">
         <f>VLOOKUP(Principal!$G$2,[1]Niveaux!$A$2:$C$21,3)</f>
-        <v>#VALUE!</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:16">

</xml_diff>